<commit_message>
Fixed soc calculation during inner iterations (previously soc would advance during inner iterations). Added polynomial approximation.
</commit_message>
<xml_diff>
--- a/python/parameters.xlsx
+++ b/python/parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -846,8 +846,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -942,15 +946,6 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -988,12 +983,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1030,6 +1034,8 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1066,6 +1072,8 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1397,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1413,22 +1421,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="20">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="H2" s="14" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="H2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5"/>
@@ -1466,7 +1474,7 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="1"/>
@@ -1480,7 +1488,7 @@
       <c r="J4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="15" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="1"/>
@@ -1494,7 +1502,7 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <v>277.54000000000002</v>
       </c>
       <c r="E5" s="2"/>
@@ -1508,7 +1516,7 @@
       <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="16">
         <v>363</v>
       </c>
       <c r="L5" s="2"/>
@@ -1517,66 +1525,66 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>0.41699999999999998</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="21">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="15">
         <v>-1</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="15">
         <v>20146.599999999999</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="27">
         <v>1E-14</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="15">
         <v>61266.35</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="19" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1588,10 +1596,10 @@
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="16">
         <v>2.02</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
@@ -1600,8 +1608,8 @@
       <c r="J8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13">
@@ -1612,10 +1620,10 @@
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <v>2.8000000000000002E-12</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="16">
         <v>11415.9</v>
       </c>
       <c r="F9" s="3"/>
@@ -1626,71 +1634,71 @@
       <c r="J9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="17">
         <v>4.7200000000000001E-12</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <v>9515</v>
       </c>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="25">
         <v>0.5</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="25">
         <v>0.5</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="M10" s="27"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="23">
         <v>5.77</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="18" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="23">
         <v>7.84</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="22"/>
+      <c r="M11" s="15" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1702,11 +1710,11 @@
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>64.400000000000006</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H12" s="4"/>
@@ -1716,11 +1724,11 @@
       <c r="J12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="18">
         <v>69.5</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="16" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1732,7 +1740,7 @@
       <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <v>3.54</v>
       </c>
       <c r="E13" s="4"/>
@@ -1746,7 +1754,7 @@
       <c r="J13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="16">
         <v>1.73</v>
       </c>
       <c r="L13" s="4"/>
@@ -1762,7 +1770,7 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="16">
         <v>0.94</v>
       </c>
       <c r="E14" s="4"/>
@@ -1774,7 +1782,7 @@
       <c r="J14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="16">
         <v>0.96</v>
       </c>
       <c r="L14" s="4"/>
@@ -1788,7 +1796,7 @@
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="16">
         <v>0.03</v>
       </c>
       <c r="E15" s="4"/>
@@ -1800,71 +1808,71 @@
       <c r="J15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="16">
         <v>0.02</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="16" thickBot="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>6.7540000000000003E-2</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="24" t="s">
+      <c r="E16" s="26"/>
+      <c r="F16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="26"/>
+      <c r="I16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="21">
         <v>7.2050000000000003E-2</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="24" t="s">
+      <c r="L16" s="26"/>
+      <c r="M16" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>0</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="22"/>
-      <c r="H17" s="22" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="19"/>
+      <c r="H17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="15">
         <v>0</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="22"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="3"/>
@@ -1874,7 +1882,7 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="16">
         <v>0.1</v>
       </c>
       <c r="E18" s="3"/>
@@ -1888,7 +1896,7 @@
       <c r="J18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="16">
         <v>0.1</v>
       </c>
       <c r="L18" s="3"/>
@@ -1904,7 +1912,7 @@
       <c r="C19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="16">
         <v>2100</v>
       </c>
       <c r="E19" s="3"/>
@@ -1918,7 +1926,7 @@
       <c r="J19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="16">
         <v>2100</v>
       </c>
       <c r="L19" s="3"/>
@@ -1934,11 +1942,11 @@
       <c r="C20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="16">
         <v>0</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="3"/>
@@ -1948,11 +1956,11 @@
       <c r="J20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="16">
         <v>0</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1964,11 +1972,11 @@
       <c r="C21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="16">
         <v>0</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="16" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="3"/>
@@ -1978,11 +1986,11 @@
       <c r="J21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="16">
         <v>0</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="19" t="s">
+      <c r="M21" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1994,7 +2002,7 @@
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="16">
         <v>0.4</v>
       </c>
       <c r="E22" s="3"/>
@@ -2006,7 +2014,7 @@
       <c r="J22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="16">
         <v>0.4</v>
       </c>
       <c r="L22" s="3"/>
@@ -2020,10 +2028,10 @@
       <c r="C23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="3" t="s">
         <v>35</v>
       </c>
@@ -2034,57 +2042,57 @@
       <c r="J23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="17">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="L23" s="19"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="16" thickBot="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27" t="s">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="21">
         <v>0</v>
       </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="21">
         <v>0</v>
       </c>
-      <c r="L24" s="24"/>
-      <c r="M24" s="27"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="26" spans="1:13" ht="20">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
-      <c r="H26" s="14" t="s">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+      <c r="H26" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="16"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="34"/>
     </row>
     <row r="27" spans="1:13" ht="16" thickBot="1">
       <c r="A27" s="5"/>
@@ -2113,66 +2121,66 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="16" thickBot="1">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="H28" s="32" t="s">
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="H28" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="I28" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="32" t="s">
+      <c r="J28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="33" t="s">
+      <c r="K28" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="23">
         <v>20</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="18" t="s">
+      <c r="E29" s="22"/>
+      <c r="F29" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="J29" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="23">
         <v>20</v>
       </c>
-      <c r="L29" s="25"/>
-      <c r="M29" s="18" t="s">
+      <c r="L29" s="22"/>
+      <c r="M29" s="15" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2184,7 +2192,7 @@
       <c r="C30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="16">
         <v>0</v>
       </c>
       <c r="E30" s="4"/>
@@ -2196,59 +2204,59 @@
       <c r="J30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="16">
         <v>0</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="1:13" ht="16" thickBot="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="24" t="s">
+      <c r="E31" s="26"/>
+      <c r="F31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29" t="s">
+      <c r="H31" s="26"/>
+      <c r="I31" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L31" s="29"/>
-      <c r="M31" s="24" t="s">
+      <c r="L31" s="26"/>
+      <c r="M31" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="20">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-      <c r="H33" s="14" t="s">
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
+      <c r="H33" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="1:13" ht="16" thickBot="1">
       <c r="A34" s="5"/>
@@ -2277,34 +2285,34 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="16" thickBot="1">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35" s="15">
         <v>30</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="18" t="s">
+      <c r="E35" s="28"/>
+      <c r="F35" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H35" s="32" t="s">
+      <c r="H35" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="32" t="s">
+      <c r="J35" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="33" t="s">
+      <c r="K35" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
@@ -2314,25 +2322,25 @@
       <c r="C36" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="16" t="s">
         <v>83</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="4"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="25" t="s">
+      <c r="I36" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="25" t="s">
+      <c r="J36" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K36" s="23">
         <v>52</v>
       </c>
-      <c r="L36" s="25"/>
-      <c r="M36" s="18" t="s">
+      <c r="L36" s="22"/>
+      <c r="M36" s="15" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2344,7 +2352,7 @@
       <c r="C37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="16">
         <v>750</v>
       </c>
       <c r="E37" s="4"/>
@@ -2358,7 +2366,7 @@
       <c r="J37" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="16">
         <v>0.55000000000000004</v>
       </c>
       <c r="L37" s="4"/>
@@ -2372,25 +2380,25 @@
       <c r="C38" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="18">
         <v>10</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29" t="s">
+      <c r="H38" s="26"/>
+      <c r="I38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J38" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K38" s="24">
+      <c r="K38" s="21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L38" s="29"/>
-      <c r="M38" s="24" t="s">
+      <c r="L38" s="26"/>
+      <c r="M38" s="21" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2402,11 +2410,11 @@
       <c r="C39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="16">
         <v>3.676E-3</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2418,7 +2426,7 @@
       <c r="C40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="16">
         <v>1000</v>
       </c>
       <c r="E40" s="4"/>
@@ -2434,10 +2442,10 @@
       <c r="C41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="16">
         <v>1</v>
       </c>
-      <c r="E41" s="19"/>
+      <c r="E41" s="16"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:13">
@@ -2448,7 +2456,7 @@
       <c r="C42" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="16">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="E42" s="4"/>
@@ -2464,7 +2472,7 @@
       <c r="C43" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="16">
         <v>4.2</v>
       </c>
       <c r="E43" s="4"/>
@@ -2473,18 +2481,18 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="16" thickBot="1">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29" t="s">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="21">
         <v>2.5</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
+      <c r="E44" s="26"/>
+      <c r="F44" s="26" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2503,7 +2511,7 @@
       <c r="D47" s="10"/>
       <c r="E47" s="11"/>
       <c r="F47" s="10"/>
-      <c r="K47" s="17"/>
+      <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="10"/>
@@ -2652,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2666,36 +2674,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="16" thickBot="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="31" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2838,13 +2846,13 @@
           <x14:formula1>
             <xm:f>Lists!$D$4:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A7</xm:sqref>
+          <xm:sqref>I3:I7 A3:A7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$E$4:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D7</xm:sqref>
+          <xm:sqref>L3:L7 D3:D7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added some parameters to the spreadsheet
</commit_message>
<xml_diff>
--- a/python/parameters.xlsx
+++ b/python/parameters.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
     <sheet name="cycle" sheetId="3" r:id="rId2"/>
     <sheet name="Lists" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,6 +27,30 @@
     <author>Ben Kenney</author>
   </authors>
   <commentList>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-1 here means that the simulation uses a diffusion factor which describes the soc dependence on D</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I17" authorId="0">
       <text>
         <r>
@@ -47,6 +72,30 @@
           </rPr>
           <t xml:space="preserve">
 3.2e-8 22189.1352</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Use either the finite difference method to solve for the concentrtion profile through the solid particles or use a 2-parameter approximation to the diffusion equation for increased speed.</t>
         </r>
       </text>
     </comment>
@@ -238,8 +287,90 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ben Kenney</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-1 here means that the simulation uses a diffusion factor which describes the soc dependence on D</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3.2e-8 22189.1352</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Use either the finite difference method to solve for the concentrtion profile through the solid particles or use a 2-parameter approximation to the diffusion equation for increased speed.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="134">
   <si>
     <t>Positive</t>
   </si>
@@ -620,6 +751,27 @@
   </si>
   <si>
     <t>Max time step</t>
+  </si>
+  <si>
+    <t>Separator thickness</t>
+  </si>
+  <si>
+    <t>Solver</t>
+  </si>
+  <si>
+    <t>Diffusion solver technique</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Finite difference</t>
+  </si>
+  <si>
+    <t>Polynomial approximation</t>
   </si>
 </sst>
 </file>
@@ -698,18 +850,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -845,8 +997,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -924,8 +1100,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -940,42 +1126,33 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -996,8 +1173,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1036,6 +1229,11 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1074,6 +1272,11 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1403,40 +1606,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M58"/>
+  <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="34"/>
+    <col min="5" max="5" width="15.5" style="34" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="34"/>
+    <col min="8" max="8" width="11.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="34"/>
+    <col min="12" max="12" width="15.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="20">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2"/>
+      <c r="H2" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5"/>
@@ -1474,7 +1682,7 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="1"/>
@@ -1488,7 +1696,7 @@
       <c r="J4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="1"/>
@@ -1502,7 +1710,7 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="11">
         <v>277.54000000000002</v>
       </c>
       <c r="E5" s="2"/>
@@ -1516,7 +1724,7 @@
       <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="11">
         <v>363</v>
       </c>
       <c r="L5" s="2"/>
@@ -1525,66 +1733,66 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <v>0.41699999999999998</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="16">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>-1</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="10">
         <v>20146.599999999999</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="22">
         <v>1E-14</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="10">
         <v>61266.35</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1596,10 +1804,10 @@
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="11">
         <v>2.02</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
@@ -1608,8 +1816,8 @@
       <c r="J8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13">
@@ -1620,10 +1828,10 @@
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="12">
         <v>2.8000000000000002E-12</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="11">
         <v>11415.9</v>
       </c>
       <c r="F9" s="3"/>
@@ -1634,71 +1842,71 @@
       <c r="J9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="12">
         <v>4.7200000000000001E-12</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="11">
         <v>9515</v>
       </c>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" ht="16" thickBot="1">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="20">
         <v>0.5</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="20">
         <v>0.5</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="24"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="18">
         <v>5.77</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="18">
         <v>7.84</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="15" t="s">
+      <c r="L11" s="17"/>
+      <c r="M11" s="10" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1710,11 +1918,11 @@
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="13">
         <v>64.400000000000006</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="11" t="s">
         <v>114</v>
       </c>
       <c r="H12" s="4"/>
@@ -1724,11 +1932,11 @@
       <c r="J12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="13">
         <v>69.5</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1740,7 +1948,7 @@
       <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="11">
         <v>3.54</v>
       </c>
       <c r="E13" s="4"/>
@@ -1754,7 +1962,7 @@
       <c r="J13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="11">
         <v>1.73</v>
       </c>
       <c r="L13" s="4"/>
@@ -1770,7 +1978,7 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="11">
         <v>0.94</v>
       </c>
       <c r="E14" s="4"/>
@@ -1782,7 +1990,7 @@
       <c r="J14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="11">
         <v>0.96</v>
       </c>
       <c r="L14" s="4"/>
@@ -1796,7 +2004,7 @@
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="11">
         <v>0.03</v>
       </c>
       <c r="E15" s="4"/>
@@ -1808,71 +2016,71 @@
       <c r="J15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="11">
         <v>0.02</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="16" thickBot="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="16">
         <v>6.7540000000000003E-2</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="16">
         <v>7.2050000000000003E-2</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="21" t="s">
+      <c r="L16" s="21"/>
+      <c r="M16" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="10">
         <v>0</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="19"/>
-      <c r="H17" s="19" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="14"/>
+      <c r="H17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="10">
         <v>0</v>
       </c>
-      <c r="L17" s="15"/>
-      <c r="M17" s="19"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="3"/>
@@ -1882,7 +2090,7 @@
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="11">
         <v>0.1</v>
       </c>
       <c r="E18" s="3"/>
@@ -1896,7 +2104,7 @@
       <c r="J18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="11">
         <v>0.1</v>
       </c>
       <c r="L18" s="3"/>
@@ -1912,7 +2120,7 @@
       <c r="C19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="11">
         <v>2100</v>
       </c>
       <c r="E19" s="3"/>
@@ -1926,7 +2134,7 @@
       <c r="J19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="11">
         <v>2100</v>
       </c>
       <c r="L19" s="3"/>
@@ -1942,11 +2150,11 @@
       <c r="C20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="11">
         <v>0</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="3"/>
@@ -1956,11 +2164,11 @@
       <c r="J20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="11">
         <v>0</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="16" t="s">
+      <c r="M20" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1972,11 +2180,11 @@
       <c r="C21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="11">
         <v>0</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="3"/>
@@ -1986,11 +2194,11 @@
       <c r="J21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="11">
         <v>0</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="16" t="s">
+      <c r="M21" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2002,7 +2210,7 @@
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="11">
         <v>0.4</v>
       </c>
       <c r="E22" s="3"/>
@@ -2014,7 +2222,7 @@
       <c r="J22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K22" s="11">
         <v>0.4</v>
       </c>
       <c r="L22" s="3"/>
@@ -2028,10 +2236,10 @@
       <c r="C23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="12">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="3" t="s">
         <v>35</v>
       </c>
@@ -2042,581 +2250,612 @@
       <c r="J23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="12">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="L23" s="16"/>
+      <c r="L23" s="11"/>
       <c r="M23" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="16" thickBot="1">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="16">
         <v>0</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="21">
+      <c r="K24" s="16">
         <v>0</v>
       </c>
-      <c r="L24" s="21"/>
-      <c r="M24" s="24"/>
-    </row>
-    <row r="26" spans="1:13" ht="20">
-      <c r="A26" s="32" t="s">
+      <c r="L24" s="16"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="1:13" ht="16" thickBot="1">
+      <c r="A25" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="24"/>
+      <c r="H25" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="L25" s="31"/>
+      <c r="M25" s="24"/>
+    </row>
+    <row r="27" spans="1:13" ht="20">
+      <c r="A27" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="H26" s="32" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="H27" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="34"/>
-    </row>
-    <row r="27" spans="1:13" ht="16" thickBot="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="s">
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="1:13" ht="16" thickBot="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="7" t="s">
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="M28" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16" thickBot="1">
-      <c r="A28" s="29" t="s">
+    <row r="29" spans="1:13" ht="16" thickBot="1">
+      <c r="A29" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C29" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D29" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="H28" s="29" t="s">
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="H29" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="29" t="s">
+      <c r="I29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J29" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="30" t="s">
+      <c r="K29" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="22" t="s">
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D30" s="18">
         <v>20</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="15" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H30" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K30" s="18">
         <v>20</v>
       </c>
-      <c r="L29" s="22"/>
-      <c r="M29" s="15" t="s">
+      <c r="L30" s="17"/>
+      <c r="M30" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:13">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D31" s="11">
         <v>0</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="16">
+      <c r="K31" s="11">
         <v>0</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" ht="16" thickBot="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26" t="s">
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" ht="16" thickBot="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C32" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D32" s="16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="21" t="s">
+      <c r="E32" s="21"/>
+      <c r="F32" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26" t="s">
+      <c r="H32" s="21"/>
+      <c r="I32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J32" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="21">
+      <c r="K32" s="16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L31" s="26"/>
-      <c r="M31" s="21" t="s">
+      <c r="L32" s="21"/>
+      <c r="M32" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="20">
-      <c r="A33" s="32" t="s">
+    <row r="34" spans="1:13" ht="20">
+      <c r="A34" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
-      <c r="H33" s="32" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="H34" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="34"/>
-    </row>
-    <row r="34" spans="1:13" ht="16" thickBot="1">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7" t="s">
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="29"/>
+    </row>
+    <row r="35" spans="1:13" ht="16" thickBot="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="7" t="s">
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="L35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="M35" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16" thickBot="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22" t="s">
+    <row r="36" spans="1:13" ht="16" thickBot="1">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C36" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D36" s="10">
         <v>30</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="15" t="s">
+      <c r="E36" s="23"/>
+      <c r="F36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H36" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="29" t="s">
+      <c r="I36" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J36" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="30" t="s">
+      <c r="K36" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="4"/>
-      <c r="H36" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I36" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="23">
-        <v>52</v>
-      </c>
-      <c r="L36" s="22"/>
-      <c r="M36" s="15" t="s">
-        <v>114</v>
-      </c>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="16">
-        <v>750</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K37" s="16">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" ht="16" thickBot="1">
+        <v>80</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="4"/>
+      <c r="H37" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="18">
+        <v>52</v>
+      </c>
+      <c r="L37" s="17"/>
+      <c r="M37" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="18">
-        <v>10</v>
+        <v>69</v>
+      </c>
+      <c r="D38" s="11">
+        <v>750</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="J38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="21">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L38" s="26"/>
-      <c r="M38" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>73</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" ht="16" thickBot="1">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="16">
-        <v>3.676E-3</v>
+        <v>71</v>
+      </c>
+      <c r="D39" s="13">
+        <v>5</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L39" s="21"/>
+      <c r="M39" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="16">
-        <v>1000</v>
+        <v>75</v>
+      </c>
+      <c r="D40" s="11">
+        <v>3.676E-3</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4" t="s">
-        <v>86</v>
+      <c r="F40" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="16">
-        <v>1</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="16">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="16">
-        <v>4.2</v>
+        <v>92</v>
+      </c>
+      <c r="D43" s="11">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16" thickBot="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26" t="s">
+    <row r="45" spans="1:13" ht="16" thickBot="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C45" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D45" s="16">
         <v>2.5</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26" t="s">
+      <c r="E45" s="21"/>
+      <c r="F45" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="20">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="10"/>
-      <c r="K47" s="14"/>
+    <row r="47" spans="1:13" ht="20">
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="10"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="36"/>
+      <c r="K48" s="38"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="10"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="H2:M2"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="K25:L25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$B$4:$B$9</xm:f>
@@ -2627,25 +2866,31 @@
           <x14:formula1>
             <xm:f>Lists!$C$4:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D49 D36</xm:sqref>
+          <xm:sqref>D50 D37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$F$4:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F11:F12 F20:F21 M11:M12 M20:M21 F29 M36 M29</xm:sqref>
+          <xm:sqref>F11:F12 F20:F21 M11:M12 M20:M21 F30 M37 M30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$G$4:$G$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F16 M16 F31 M31 F39 M38</xm:sqref>
+          <xm:sqref>F16 M16 F32 M32 F40 M39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$H$4:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F35</xm:sqref>
+          <xm:sqref>F36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$I$4:$I$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D25 K25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2660,8 +2905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2674,36 +2919,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="16" thickBot="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="26" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2865,15 +3110,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H9"/>
+  <dimension ref="B3:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -2895,8 +3140,11 @@
       <c r="H3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="I3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -2918,8 +3166,11 @@
       <c r="H4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="I4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>26</v>
       </c>
@@ -2941,8 +3192,11 @@
       <c r="H5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="I5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -2956,7 +3210,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -2970,7 +3224,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -2978,7 +3232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -2991,4 +3245,1182 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:13" ht="20">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" ht="31" thickBot="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11">
+        <v>277.54000000000002</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="11">
+        <v>363</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" thickBot="1">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>20146.599999999999</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="22">
+        <v>1E-14</v>
+      </c>
+      <c r="L7" s="10">
+        <v>61266.35</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2.02</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2.8000000000000002E-12</v>
+      </c>
+      <c r="E9" s="11">
+        <v>11415.9</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>4.7200000000000001E-12</v>
+      </c>
+      <c r="L9" s="11">
+        <v>9515</v>
+      </c>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" thickBot="1">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="18">
+        <v>5.77</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="18">
+        <v>7.84</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="13">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="13">
+        <v>69.5</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3.54</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="11">
+        <v>1.73</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.94</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.96</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" thickBot="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="16">
+        <v>6.7540000000000003E-2</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="16">
+        <v>7.2050000000000003E-2</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="14"/>
+      <c r="H17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2100</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K19" s="11">
+        <v>2100</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="12">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="12">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16" thickBot="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="16">
+        <v>0</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="1:13" ht="16" thickBot="1">
+      <c r="A25" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="33"/>
+      <c r="H25" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="L25" s="31"/>
+      <c r="M25" s="33"/>
+    </row>
+    <row r="27" spans="1:13" ht="20">
+      <c r="A27" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="H27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="1:13" ht="31" thickBot="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16" thickBot="1">
+      <c r="A29" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="H29" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="18">
+        <v>20</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="18">
+        <v>20</v>
+      </c>
+      <c r="L30" s="17"/>
+      <c r="M30" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K31" s="11">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" ht="16" thickBot="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L32" s="21"/>
+      <c r="M32" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="20">
+      <c r="A34" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="H34" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="29"/>
+    </row>
+    <row r="35" spans="1:13" ht="31" thickBot="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="16" thickBot="1">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="10">
+        <v>30</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="4"/>
+      <c r="H37" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="18">
+        <v>52</v>
+      </c>
+      <c r="L37" s="17"/>
+      <c r="M37" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="11">
+        <v>750</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" ht="16" thickBot="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="13">
+        <v>10</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L39" s="21"/>
+      <c r="M39" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="11">
+        <v>3.676E-3</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="16" thickBot="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="H27:M27"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$I$4:$I$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D25 K25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$H$4:$H$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$G$4:$G$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F16 M16 F32 M32 F40 M39</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$F$4:$F$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F11:F12 F20:F21 M11:M12 M20:M21 F30 M37 M30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$C$4:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$B$4:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4 K4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added geometry worksheet to parameters. Cleaned up some SPM code.
</commit_message>
<xml_diff>
--- a/python/parameters.xlsx
+++ b/python/parameters.xlsx
@@ -4,14 +4,84 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
     <sheet name="cycle" sheetId="3" r:id="rId2"/>
     <sheet name="Lists" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Cell Properties" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Cell Properties'!$I$4:$I$9</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Cell Properties'!$I$4</definedName>
+    <definedName name="solver_lhs10" localSheetId="3" hidden="1">'Cell Properties'!$I$8</definedName>
+    <definedName name="solver_lhs11" localSheetId="3" hidden="1">'Cell Properties'!$I$9</definedName>
+    <definedName name="solver_lhs12" localSheetId="3" hidden="1">'Cell Properties'!$I$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="3" hidden="1">'Cell Properties'!$J$6</definedName>
+    <definedName name="solver_lhs14" localSheetId="3" hidden="1">'Cell Properties'!$J$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Cell Properties'!$I$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Cell Properties'!$I$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs7" localSheetId="3" hidden="1">'Cell Properties'!$I$7</definedName>
+    <definedName name="solver_lhs8" localSheetId="3" hidden="1">'Cell Properties'!$I$7</definedName>
+    <definedName name="solver_lhs9" localSheetId="3" hidden="1">'Cell Properties'!$I$8</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">14</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Cell Properties'!$I$12</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel13" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel14" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">10</definedName>
+    <definedName name="solver_rhs10" localSheetId="3" hidden="1">0.85</definedName>
+    <definedName name="solver_rhs11" localSheetId="3" hidden="1">0.98</definedName>
+    <definedName name="solver_rhs12" localSheetId="3" hidden="1">0.9</definedName>
+    <definedName name="solver_rhs13" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs14" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">20</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'Cell Properties'!$J$5</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">20</definedName>
+    <definedName name="solver_rhs7" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rhs8" localSheetId="3" hidden="1">0.5</definedName>
+    <definedName name="solver_rhs9" localSheetId="3" hidden="1">0.98</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -183,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="F2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="I2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,78 +360,282 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Ben Kenney</author>
+    <author>Dana</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
           </rPr>
-          <t>Ben Kenney:</t>
+          <t xml:space="preserve">Dana:
+</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
--1 here means that the simulation uses a diffusion factor which describes the soc dependence on D</t>
+          <t>Calculation includes thickness of folded electrodes + thickness of casing. Does NOT include thickness from any spacers inside of cell</t>
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
           </rPr>
-          <t>Ben Kenney:</t>
+          <t>Dana:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-3.2e-8 22189.1352</t>
+The number of folds that the electrode undergoes to pack everything into the overall cell dimensions. This is normally unknown (can be found by dissasembling cells). Change this number until it matches other known values such as cell thickness or cell mass.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0">
+    <comment ref="B62" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
           </rPr>
-          <t>Ben Kenney:</t>
+          <t>Dana:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Use either the finite difference method to solve for the concentrtion profile through the solid particles or use a 2-parameter approximation to the diffusion equation for increased speed.</t>
+Width of unrolled/unpacked electrode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E62" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Width of unrolled/unpacked electrode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Width of unrolled/unpacked electrode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Width of unrolled/unpacked electrode</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Note: Coating is double sided, so this is 2*actual thickness</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Note: Coating is double sided, so this is 2*actual thickness</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B83" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cast density including porosity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E83" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cast density including porosity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B84" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cast density without porosity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E84" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dana:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cast density without porosity</t>
         </r>
       </text>
     </comment>
@@ -370,7 +644,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="228">
   <si>
     <t>Positive</t>
   </si>
@@ -750,9 +1024,6 @@
     <t>rhos</t>
   </si>
   <si>
-    <t>Max time step</t>
-  </si>
-  <si>
     <t>Separator thickness</t>
   </si>
   <si>
@@ -772,13 +1043,302 @@
   </si>
   <si>
     <t>Polynomial approximation</t>
+  </si>
+  <si>
+    <t>Units1</t>
+  </si>
+  <si>
+    <t>Units2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>Step Type Index</t>
+  </si>
+  <si>
+    <t>Stop Type Index</t>
+  </si>
+  <si>
+    <t>Max Time Step</t>
+  </si>
+  <si>
+    <t>Values in grey are calcualted, all other values are user inputs</t>
+  </si>
+  <si>
+    <t>Overall Cell Dimensions</t>
+  </si>
+  <si>
+    <t>Volt Cell</t>
+  </si>
+  <si>
+    <t>Electrovaya Cell</t>
+  </si>
+  <si>
+    <t>Width (mm)</t>
+  </si>
+  <si>
+    <t>Height (mm)</t>
+  </si>
+  <si>
+    <t>Thickness (mm)</t>
+  </si>
+  <si>
+    <t>Cell mass (kg)</t>
+  </si>
+  <si>
+    <t>Number of folds</t>
+  </si>
+  <si>
+    <t>Electrode Formula &amp; Material Properties</t>
+  </si>
+  <si>
+    <t>Positive Electrode</t>
+  </si>
+  <si>
+    <t>Bulk Density</t>
+  </si>
+  <si>
+    <t>Thermal conductivity</t>
+  </si>
+  <si>
+    <t>mass fraction (solids)</t>
+  </si>
+  <si>
+    <t>volume fraction</t>
+  </si>
+  <si>
+    <t>W/m/K</t>
+  </si>
+  <si>
+    <t>(solids basis)</t>
+  </si>
+  <si>
+    <t>(total volume basis)</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>PVDF</t>
+  </si>
+  <si>
+    <t>Pore / Electrolyte</t>
+  </si>
+  <si>
+    <t>Negative Electrode</t>
+  </si>
+  <si>
+    <t>Graphite</t>
+  </si>
+  <si>
+    <t>Dimensions &amp; Properties</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>(microns)</t>
+  </si>
+  <si>
+    <t>Casing</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Pouch cell casing</t>
+  </si>
+  <si>
+    <t>Density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>Heat Capacity (J/kg/K)</t>
+  </si>
+  <si>
+    <t>Thermal conductivity (W/kg/K)</t>
+  </si>
+  <si>
+    <t>Volume (m^3)</t>
+  </si>
+  <si>
+    <t>Mass (kg)</t>
+  </si>
+  <si>
+    <t>Positive Electrode Side</t>
+  </si>
+  <si>
+    <t>Negative Electrode Side</t>
+  </si>
+  <si>
+    <t>Tab Dimensions</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Thickness (microns)</t>
+  </si>
+  <si>
+    <t>Heat capacity (J/kg/K)</t>
+  </si>
+  <si>
+    <t>Thermal conductivity (W/m/K)</t>
+  </si>
+  <si>
+    <t>Foil Dimensions</t>
+  </si>
+  <si>
+    <t>Foil thickness (microns)</t>
+  </si>
+  <si>
+    <t>Bulk Density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>Electrode Dimensions</t>
+  </si>
+  <si>
+    <t>Desciption</t>
+  </si>
+  <si>
+    <t>(see electrode formulation)</t>
+  </si>
+  <si>
+    <t>Cast Properties</t>
+  </si>
+  <si>
+    <t>Apparent Density (g/cm^3)</t>
+  </si>
+  <si>
+    <t>Bulk density (g/cm^3)</t>
+  </si>
+  <si>
+    <t>Electrode Properties (cast+foil+tab)</t>
+  </si>
+  <si>
+    <t>Tot volume (m^3)</t>
+  </si>
+  <si>
+    <t>Tot mass (kg)</t>
+  </si>
+  <si>
+    <t>Avg density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>Avg heat capacity (J/Kg/K)</t>
+  </si>
+  <si>
+    <t>Avg thermal conductivity (W/m/K)</t>
+  </si>
+  <si>
+    <t>Cell Properties</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Mass fraction</t>
+  </si>
+  <si>
+    <t>Volume fraction</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Electrode folds</t>
+  </si>
+  <si>
+    <t>Single fold thickness</t>
+  </si>
+  <si>
+    <t>microns</t>
+  </si>
+  <si>
+    <t>Cell thickness (just electrodes)</t>
+  </si>
+  <si>
+    <t>Cell thickness (with casing)</t>
+  </si>
+  <si>
+    <t>Cell avg heat capacity</t>
+  </si>
+  <si>
+    <t>Cell avg density</t>
+  </si>
+  <si>
+    <t>Cell avg thermal conductivity</t>
+  </si>
+  <si>
+    <t>Cell weight</t>
+  </si>
+  <si>
+    <t>SBLiMotive</t>
+  </si>
+  <si>
+    <t>Al casing</t>
+  </si>
+  <si>
+    <t>num fold</t>
+  </si>
+  <si>
+    <t>pos thickness</t>
+  </si>
+  <si>
+    <t>neg thickness</t>
+  </si>
+  <si>
+    <t>casing thickness</t>
+  </si>
+  <si>
+    <t>Fitting parameters</t>
+  </si>
+  <si>
+    <t>Wt % pos</t>
+  </si>
+  <si>
+    <t>Wt % neg</t>
+  </si>
+  <si>
+    <t>sse</t>
+  </si>
+  <si>
+    <t>Wt % pos c</t>
+  </si>
+  <si>
+    <t>Wt % neg c</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -822,8 +1382,39 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -860,8 +1451,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1009,20 +1606,151 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1110,8 +1838,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1160,25 +1902,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1189,8 +1913,131 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1234,6 +2081,13 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1277,6 +2131,13 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1608,43 +2469,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="34"/>
-    <col min="5" max="5" width="15.5" style="34" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="34"/>
-    <col min="8" max="8" width="11.83203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="34"/>
-    <col min="12" max="12" width="15.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="34"/>
+    <col min="1" max="1" width="11.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="27"/>
+    <col min="5" max="5" width="15.5" style="27" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="27"/>
+    <col min="8" max="8" width="11.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="27"/>
+    <col min="12" max="12" width="15.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="20">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
       <c r="G2"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5"/>
@@ -2285,52 +3146,52 @@
       <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:13" ht="16" thickBot="1">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="C25" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="31"/>
+      <c r="D25" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="48"/>
       <c r="F25" s="24"/>
       <c r="H25" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="J25" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="K25" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" s="31"/>
+      <c r="K25" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="L25" s="48"/>
       <c r="M25" s="24"/>
     </row>
     <row r="27" spans="1:13" ht="20">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="H27" s="27" t="s">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="47"/>
+      <c r="H27" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="29"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="47"/>
     </row>
     <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="5"/>
@@ -2479,22 +3340,22 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="20">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="H34" s="27" t="s">
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="47"/>
+      <c r="H34" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="29"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="47"/>
     </row>
     <row r="35" spans="1:13" ht="16" thickBot="1">
       <c r="A35" s="5"/>
@@ -2561,7 +3422,7 @@
         <v>80</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="4"/>
@@ -2569,7 +3430,7 @@
         <v>31</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J37" s="17" t="s">
         <v>5</v>
@@ -2590,8 +3451,9 @@
       <c r="C38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="11">
-        <v>750</v>
+      <c r="D38" s="105">
+        <f>'Cell Properties'!C108</f>
+        <v>885.13366342599079</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
@@ -2735,111 +3597,112 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="20">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="36"/>
-      <c r="K48" s="38"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="29"/>
+      <c r="K48" s="31"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="36"/>
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="36"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="H2:M2"/>
@@ -2903,183 +3766,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="36" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:10" ht="20">
+      <c r="A1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" thickBot="1">
-      <c r="A2" s="26" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickBot="1">
+      <c r="A2" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="H2" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="37">
         <f>MATCH(A3,Lists!$D$4:$D$5,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>-0.88</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="37">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D3" s="40" t="str">
+        <f>VLOOKUP(A3,Lists!$D$4:$J$5,7)</f>
+        <v>A</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="E3">
-        <f>MATCH(D3,Lists!$E$4:$E$8,FALSE)-1</f>
+      <c r="F3" s="38">
+        <f>MATCH(E3,Lists!$E$4:$E$8,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="G3" s="38">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="H3" s="43" t="str">
+        <f>VLOOKUP(E3,Lists!$E$4:$K$8,7,FALSE)</f>
+        <v>V</v>
+      </c>
+      <c r="I3" s="37">
+        <v>50</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="37">
         <f>MATCH(A4,Lists!$D$4:$D$5,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="37">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="40" t="str">
+        <f>VLOOKUP(A4,Lists!$D$4:$J$5,7)</f>
+        <v>A</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="E4">
-        <f>MATCH(D4,Lists!$E$4:$E$8,FALSE)-1</f>
+      <c r="F4" s="38">
+        <f>MATCH(E4,Lists!$E$4:$E$8,FALSE)-1</f>
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="38">
         <v>600</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="43" t="str">
+        <f>VLOOKUP(E4,Lists!$E$4:$K$8,7,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="I4" s="37">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="J4" s="37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="37">
         <f>MATCH(A5,Lists!$D$4:$D$5,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="37">
         <v>0.88</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="40" t="str">
+        <f>VLOOKUP(A5,Lists!$D$4:$J$5,7)</f>
+        <v>A</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="E5">
-        <f>MATCH(D5,Lists!$E$4:$E$8,FALSE)-1</f>
+      <c r="F5" s="38">
+        <f>MATCH(E5,Lists!$E$4:$E$8,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="G5" s="38">
         <v>4.2</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="43" t="str">
+        <f>VLOOKUP(E5,Lists!$E$4:$K$8,7,FALSE)</f>
+        <v>V</v>
+      </c>
+      <c r="I5" s="37">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="J5" s="37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="37">
         <f>MATCH(A6,Lists!$D$4:$D$5,FALSE)-1</f>
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="37">
         <v>4.2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="40" t="str">
+        <f>VLOOKUP(A6,Lists!$D$4:$J$5,7)</f>
+        <v>V</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E6">
-        <f>MATCH(D6,Lists!$E$4:$E$8,FALSE)-1</f>
+      <c r="F6" s="38">
+        <f>MATCH(E6,Lists!$E$4:$E$8,FALSE)-1</f>
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="38">
         <v>0.01</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="43" t="str">
+        <f>VLOOKUP(E6,Lists!$E$4:$K$8,7,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="I6" s="37">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="J6" s="37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="37">
         <f>MATCH(A7,Lists!$D$4:$D$5,FALSE)-1</f>
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="37">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="40" t="str">
+        <f>VLOOKUP(A7,Lists!$D$4:$J$5,7)</f>
+        <v>A</v>
+      </c>
+      <c r="E7" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="E7">
-        <f>MATCH(D7,Lists!$E$4:$E$8,FALSE)-1</f>
+      <c r="F7" s="38">
+        <f>MATCH(E7,Lists!$E$4:$E$8,FALSE)-1</f>
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="G7" s="38">
         <v>600</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="43" t="str">
+        <f>VLOOKUP(E7,Lists!$E$4:$K$8,7,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="I7" s="37">
         <v>50</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3091,13 +4026,13 @@
           <x14:formula1>
             <xm:f>Lists!$D$4:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I7 A3:A7</xm:sqref>
+          <xm:sqref>K3:K7 A3:A7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$E$4:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L7 D3:D7</xm:sqref>
+          <xm:sqref>N3:N7 E3:E7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3110,15 +4045,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I9"/>
+  <dimension ref="B3:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -3141,10 +4076,16 @@
         <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+        <v>130</v>
+      </c>
+      <c r="J3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -3167,10 +4108,19 @@
         <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
+        <v>131</v>
+      </c>
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>26</v>
       </c>
@@ -3193,10 +4143,19 @@
         <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
+        <v>132</v>
+      </c>
+      <c r="J5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -3209,8 +4168,14 @@
       <c r="G6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="K6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -3223,22 +4188,35 @@
       <c r="G7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="K7" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="K8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3249,1175 +4227,1645 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M45"/>
+  <dimension ref="B1:J111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="20">
-      <c r="A2" s="27" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" s="50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="H3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="20">
+      <c r="B4" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4">
+        <v>62.493806271103288</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="99">
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <v>127</v>
+      </c>
+      <c r="E5">
+        <v>145</v>
+      </c>
+      <c r="F5">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5">
+        <v>71.428571428571445</v>
+      </c>
+      <c r="J5">
+        <f>I5*1.4</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="99">
+        <v>148</v>
+      </c>
+      <c r="D6">
+        <v>177</v>
+      </c>
+      <c r="E6">
+        <v>192</v>
+      </c>
+      <c r="F6">
+        <v>148</v>
+      </c>
+      <c r="H6" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6" s="56">
+        <f>F20-F19</f>
+        <v>-2.9999999928698173E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="H7" t="s">
+        <v>219</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="56">
+        <f>F29-F28</f>
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="H2" s="27" t="s">
+    </row>
+    <row r="8" spans="2:10">
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8">
+        <v>0.88000002999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="52">
+        <f>C107</f>
+        <v>26.488545271999985</v>
+      </c>
+      <c r="D9">
+        <v>26.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="53">
+        <f>C111</f>
+        <v>1.0404832045085801</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="C11" s="54"/>
+      <c r="H11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="103">
+        <f>I4</f>
+        <v>62.493806271103288</v>
+      </c>
+      <c r="H12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I12" s="106">
+        <f>(C9-D9)^2+(C10-D10)^2</f>
+        <v>8.4511702895127896E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="C13" s="103"/>
+      <c r="I13" s="106"/>
+    </row>
+    <row r="14" spans="2:10" ht="20">
+      <c r="B14" s="51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="59">
+        <v>4750</v>
+      </c>
+      <c r="D18" s="99">
+        <v>1172</v>
+      </c>
+      <c r="E18" s="99">
+        <v>5</v>
+      </c>
+      <c r="F18" s="101">
+        <f>I8</f>
+        <v>0.88000002999999993</v>
+      </c>
+      <c r="G18" s="57">
+        <f>(F18/C18)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.74725341099764386</v>
+      </c>
+      <c r="H18" s="57">
+        <f>G18*(1-$C$85)</f>
+        <v>0.65583160130526308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="58">
+        <v>2100</v>
+      </c>
+      <c r="D19" s="99">
+        <v>710</v>
+      </c>
+      <c r="E19" s="99">
+        <v>100</v>
+      </c>
+      <c r="F19" s="101">
+        <f>I10</f>
+        <v>0.06</v>
+      </c>
+      <c r="G19" s="57">
+        <f>(F19/C19)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.11524199939073732</v>
+      </c>
+      <c r="H19" s="57">
+        <f>G19*(1-$C$85)</f>
+        <v>0.10114285714285713</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="59">
+        <v>1760</v>
+      </c>
+      <c r="D20" s="99">
+        <v>2500</v>
+      </c>
+      <c r="E20" s="99">
+        <v>1</v>
+      </c>
+      <c r="F20" s="102">
+        <f>1-F18-F19</f>
+        <v>5.9999970000000069E-2</v>
+      </c>
+      <c r="G20" s="57">
+        <f>(F20/C20)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.13750458961161893</v>
+      </c>
+      <c r="H20" s="57">
+        <f>G20*(1-$C$85)</f>
+        <v>0.12068175784090925</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="59">
+        <v>1204</v>
+      </c>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57">
+        <f>$C$85</f>
+        <v>0.12234378371097065</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="C22" s="60"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="61"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="C23" s="60"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="61"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="59">
+        <v>2100</v>
+      </c>
+      <c r="D27" s="99">
+        <v>710</v>
+      </c>
+      <c r="E27" s="99">
+        <v>100</v>
+      </c>
+      <c r="F27" s="101">
+        <f>I9</f>
+        <v>0.9</v>
+      </c>
+      <c r="G27" s="57">
+        <f>(F27/C27)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>0.89138998311761397</v>
+      </c>
+      <c r="H27" s="57">
+        <f>G27*(1-$F$85)</f>
+        <v>0.74142857142857155</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="58">
+        <v>2100</v>
+      </c>
+      <c r="D28" s="99">
+        <v>710</v>
+      </c>
+      <c r="E28" s="99">
+        <v>100</v>
+      </c>
+      <c r="F28" s="101">
+        <v>0.05</v>
+      </c>
+      <c r="G28" s="57">
+        <f>(F28/C28)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>4.9521665728756332E-2</v>
+      </c>
+      <c r="H28" s="57">
+        <f>G28*(1-$F$85)</f>
+        <v>4.1190476190476194E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="59">
+        <v>1760</v>
+      </c>
+      <c r="D29" s="99">
+        <v>2500</v>
+      </c>
+      <c r="E29" s="99">
+        <v>1</v>
+      </c>
+      <c r="F29" s="102">
+        <f>1-F27-F28</f>
+        <v>4.9999999999999975E-2</v>
+      </c>
+      <c r="G29" s="57">
+        <f>(F29/C29)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>5.9088351153629683E-2</v>
+      </c>
+      <c r="H29" s="57">
+        <f>G29*(1-$F$85)</f>
+        <v>4.9147727272727253E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="59">
+        <v>1204</v>
+      </c>
+      <c r="D30" s="60"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="57">
+        <f>$F$85</f>
+        <v>0.16823322510822503</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" s="60"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+    </row>
+    <row r="33" spans="2:8" ht="20">
+      <c r="B33" s="51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="20">
+      <c r="B34" s="51"/>
+      <c r="C34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="99">
+        <v>1324</v>
+      </c>
+      <c r="D36" s="99">
+        <v>2000</v>
+      </c>
+      <c r="E36" s="99">
+        <v>0.83</v>
+      </c>
+      <c r="F36" s="100">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G36" s="99">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="50"/>
+      <c r="F37" s="62"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="50"/>
+      <c r="F38" s="62"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="62"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" t="s">
+        <v>215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" s="62"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="99">
+        <f>I7</f>
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="62"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" s="98">
+        <v>2700</v>
+      </c>
+      <c r="D42" s="99">
+        <v>1150</v>
+      </c>
+      <c r="F42" s="62"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="98">
+        <v>870</v>
+      </c>
+      <c r="D43" s="99">
+        <v>1900</v>
+      </c>
+      <c r="F43" s="62"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="98">
+        <v>200</v>
+      </c>
+      <c r="D44" s="99">
+        <v>0.16</v>
+      </c>
+      <c r="F44" s="62"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="64">
+        <f>(C5/1000*C6/1000*2+C6/1000*C9/1000*2)*C41/1000</f>
+        <v>1.7388304700256E-5</v>
+      </c>
+      <c r="D45" s="99"/>
+      <c r="F45" s="62"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="64">
+        <f>C42*C45</f>
+        <v>4.6948422690691202E-2</v>
+      </c>
+      <c r="D46" s="99"/>
+      <c r="F46" s="62"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="82"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="F48" s="82"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="84"/>
+      <c r="E49" s="83" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="84"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="84" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="97">
+        <v>10</v>
+      </c>
+      <c r="E51" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="F51" s="97">
+        <v>10</v>
+      </c>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="97">
+        <v>25</v>
+      </c>
+      <c r="E52" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="97">
+        <v>25</v>
+      </c>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="97">
+        <v>20</v>
+      </c>
+      <c r="D53" s="67"/>
+      <c r="E53" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="97">
+        <v>20</v>
+      </c>
+      <c r="G53" s="67"/>
+      <c r="H53" s="67"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="98">
+        <v>2700</v>
+      </c>
+      <c r="E54" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="F54" s="98">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="98">
+        <v>870</v>
+      </c>
+      <c r="E55" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="F55" s="98">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="98">
+        <v>200</v>
+      </c>
+      <c r="E56" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="97">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="89">
+        <f>C51/1000*C52/1000*C53/1000000</f>
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="E57" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" s="89">
+        <f>F51/1000*F52/1000*F53/1000000</f>
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="C58" s="89">
+        <f>C57*C54</f>
+        <v>1.3499999999999999E-5</v>
+      </c>
+      <c r="E58" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" s="89">
+        <f>F57*F54</f>
+        <v>4.5000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="87"/>
+      <c r="C59" s="88"/>
+      <c r="E59" s="87"/>
+      <c r="F59" s="88"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="84"/>
+      <c r="E60" s="83" t="s">
+        <v>183</v>
+      </c>
+      <c r="F60" s="84"/>
+      <c r="G60" s="67"/>
+      <c r="H60" s="67"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="E61" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="84" t="s">
+        <v>179</v>
+      </c>
+      <c r="G61" s="67"/>
+      <c r="H61" s="67"/>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="104">
+        <f>C5*C12</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="E62" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="104">
+        <f>C5*C12</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="G62" s="67"/>
+      <c r="H62" s="67"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="104">
+        <f>C6</f>
+        <v>148</v>
+      </c>
+      <c r="E63" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="104">
+        <f>C6</f>
+        <v>148</v>
+      </c>
+      <c r="G63" s="67"/>
+      <c r="H63" s="67"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="87" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="98">
+        <v>20</v>
+      </c>
+      <c r="E64" s="87" t="s">
+        <v>184</v>
+      </c>
+      <c r="F64" s="98">
+        <v>20</v>
+      </c>
+      <c r="G64" s="67"/>
+      <c r="H64" s="67"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="97">
+        <v>2700</v>
+      </c>
+      <c r="E65" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="F65" s="98">
+        <v>9000</v>
+      </c>
+      <c r="G65" s="67"/>
+      <c r="H65" s="67"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="98">
+        <v>870</v>
+      </c>
+      <c r="E66" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="F66" s="98">
+        <v>381</v>
+      </c>
+      <c r="G66" s="67"/>
+      <c r="H66" s="67"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="98">
+        <v>200</v>
+      </c>
+      <c r="E67" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="F67" s="97">
+        <v>380</v>
+      </c>
+      <c r="G67" s="67"/>
+      <c r="H67" s="67"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" s="89">
+        <f>C62/1000*C63/1000*C64/1000000</f>
+        <v>1.6833331657184382E-5</v>
+      </c>
+      <c r="E68" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="F68" s="89">
+        <f>F62/1000*F63/1000*F64/1000000</f>
+        <v>1.6833331657184382E-5</v>
+      </c>
+      <c r="G68" s="67"/>
+      <c r="H68" s="67"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" s="89">
+        <f>C68*C65</f>
+        <v>4.5449995474397833E-2</v>
+      </c>
+      <c r="E69" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="F69" s="89">
+        <f>F68*F65</f>
+        <v>0.15149998491465944</v>
+      </c>
+      <c r="G69" s="67"/>
+      <c r="H69" s="67"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="87"/>
+      <c r="C70" s="88"/>
+      <c r="E70" s="87"/>
+      <c r="F70" s="88"/>
+      <c r="G70" s="67"/>
+      <c r="H70" s="67"/>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="84"/>
+      <c r="E71" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="F71" s="84"/>
+      <c r="G71" s="67"/>
+      <c r="H71" s="67"/>
+    </row>
+    <row r="72" spans="2:8" ht="30">
+      <c r="B72" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" s="96" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" s="85" t="s">
+        <v>187</v>
+      </c>
+      <c r="F72" s="96" t="s">
+        <v>188</v>
+      </c>
+      <c r="G72" s="67"/>
+      <c r="H72" s="67"/>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="104">
+        <f>C62</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="E73" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="F73" s="104">
+        <f>F62</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="G73" s="67"/>
+      <c r="H73" s="67"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="104">
+        <f>C63</f>
+        <v>148</v>
+      </c>
+      <c r="E74" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="F74" s="104">
+        <f>F63</f>
+        <v>148</v>
+      </c>
+      <c r="G74" s="67"/>
+      <c r="H74" s="67"/>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="B75" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" s="98">
+        <f>2*I5</f>
+        <v>142.85714285714289</v>
+      </c>
+      <c r="E75" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="F75" s="98">
+        <f>2*I6</f>
+        <v>200</v>
+      </c>
+      <c r="G75" s="68"/>
+      <c r="H75" s="68"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="90">
+        <f>(C18*H18+H19*C19+C20*H20+C21*H21)</f>
+        <v>3687.3019155880088</v>
+      </c>
+      <c r="E76" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="F76" s="90">
+        <f>(H27*C27+C28*H28+H29*C29+H30*C30)</f>
+        <v>1932.552803030303</v>
+      </c>
+      <c r="G76" s="68"/>
+      <c r="H76" s="68"/>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="B77" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="89">
+        <f>C73/1000*C74/1000*C75/1000000</f>
+        <v>1.2023808326560274E-4</v>
+      </c>
+      <c r="E77" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="F77" s="89">
+        <f>F73/1000*F74/1000*F75/1000000</f>
+        <v>1.683333165718438E-4</v>
+      </c>
+      <c r="G77" s="68"/>
+      <c r="H77" s="68"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="C78" s="89">
+        <f>C77*C76</f>
+        <v>0.44335411475188752</v>
+      </c>
+      <c r="E78" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="F78" s="89">
+        <f>F77*F76</f>
+        <v>0.32531302278430407</v>
+      </c>
+      <c r="G78" s="68"/>
+      <c r="H78" s="68"/>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="90">
+        <f>D18*H18+D19*H19+D20*H20</f>
+        <v>1142.1504599034699</v>
+      </c>
+      <c r="E79" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="F79" s="90">
+        <f>H27*D27+H28*D28+H29*D29</f>
+        <v>678.52884199134201</v>
+      </c>
+      <c r="G79" s="68"/>
+      <c r="H79" s="68"/>
+    </row>
+    <row r="80" spans="2:8">
+      <c r="B80" s="87" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="90">
+        <f>E18*H18+E19*H19+E20*H20</f>
+        <v>13.514125478652939</v>
+      </c>
+      <c r="E80" s="87" t="s">
+        <v>153</v>
+      </c>
+      <c r="F80" s="90">
+        <f>H27*E27+H28*E28+H29*E29</f>
+        <v>78.311052489177499</v>
+      </c>
+      <c r="G80" s="68"/>
+      <c r="H80" s="68"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="87"/>
+      <c r="C81" s="88"/>
+      <c r="E81" s="87"/>
+      <c r="F81" s="88"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="84"/>
+      <c r="E82" s="91" t="s">
+        <v>189</v>
+      </c>
+      <c r="F82" s="84"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" s="97">
+        <f>parameters!D13</f>
+        <v>3.54</v>
+      </c>
+      <c r="E83" s="87" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="97">
+        <f>parameters!K13</f>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="B84" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="90">
+        <f>(C18*G18+C19*G19+C20*G20)/1000</f>
+        <v>4.0334699786758064</v>
+      </c>
+      <c r="E84" s="87" t="s">
+        <v>191</v>
+      </c>
+      <c r="F84" s="90">
+        <f>(C27*G27+C28*G28+C29*G29)/1000</f>
+        <v>2.0799099606077656</v>
+      </c>
+      <c r="G84" s="70"/>
+      <c r="H84" s="70"/>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="B85" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="92">
+        <f>1-C83/C84</f>
+        <v>0.12234378371097065</v>
+      </c>
+      <c r="E85" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85" s="92">
+        <f>1-F83/F84</f>
+        <v>0.16823322510822503</v>
+      </c>
+      <c r="G85" s="56"/>
+      <c r="H85" s="56"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="87"/>
+      <c r="C86" s="93"/>
+      <c r="E86" s="87"/>
+      <c r="F86" s="93"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="56"/>
+    </row>
+    <row r="87" spans="2:9">
+      <c r="B87" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" s="84"/>
+      <c r="E87" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="F87" s="84"/>
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="89">
+        <f>C57+C68+C77</f>
+        <v>1.3707641492278713E-4</v>
+      </c>
+      <c r="E88" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="F88" s="89">
+        <f>F57+F68+F77</f>
+        <v>1.8517164822902819E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9">
+      <c r="B89" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" s="89">
+        <f>C58+C69+C78</f>
+        <v>0.48881761022628534</v>
+      </c>
+      <c r="E89" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="F89" s="89">
+        <f>F58+F69+F78</f>
+        <v>0.47685800769896347</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9">
+      <c r="B90" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" s="90">
+        <f>C89/C88</f>
+        <v>3566.0227217178694</v>
+      </c>
+      <c r="E90" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="F90" s="90">
+        <f>F89/F88</f>
+        <v>2575.2214891405251</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="B91" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="C91" s="90">
+        <f>C79*(C78/$C$89)+C66*(C69/$C$89)+C55*(C58/$C$89)</f>
+        <v>1116.8385420360898</v>
+      </c>
+      <c r="E91" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="F91" s="90">
+        <f>F79*(F78/$F$89)+F66*(F69/$F$89)+F55*(F58/$F$89)</f>
+        <v>583.97448169271343</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9">
+      <c r="B92" s="94" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" s="95">
+        <f>C80*(C78/$C$89)+C67*(C69/$C$89)+C56*(C58/$C$89)</f>
+        <v>30.858630944435109</v>
+      </c>
+      <c r="E92" s="94" t="s">
+        <v>197</v>
+      </c>
+      <c r="F92" s="95">
+        <f>F80*(F78/$F$89)+F67*(F69/$F$89)+F56*(F58/$F$89)</f>
+        <v>174.18749004773349</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="B95" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="C96" t="s">
+        <v>199</v>
+      </c>
+      <c r="D96" t="s">
+        <v>200</v>
+      </c>
+      <c r="E96" t="s">
+        <v>201</v>
+      </c>
+      <c r="F96" t="s">
+        <v>202</v>
+      </c>
+      <c r="G96" t="s">
+        <v>42</v>
+      </c>
+      <c r="H96" t="s">
+        <v>68</v>
+      </c>
+      <c r="I96" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9">
+      <c r="C97" t="s">
+        <v>203</v>
+      </c>
+      <c r="D97" t="s">
+        <v>204</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+      <c r="F97" t="s">
+        <v>135</v>
+      </c>
+      <c r="G97" t="s">
+        <v>36</v>
+      </c>
+      <c r="H97" t="s">
+        <v>73</v>
+      </c>
+      <c r="I97" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9">
+      <c r="B98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="64">
+        <f>C88</f>
+        <v>1.3707641492278713E-4</v>
+      </c>
+      <c r="D98" s="64">
+        <f>C89</f>
+        <v>0.48881761022628534</v>
+      </c>
+      <c r="E98" s="53">
+        <f>D98/SUM($D$98:$D$101)</f>
+        <v>0.46979865519035813</v>
+      </c>
+      <c r="F98" s="53">
+        <f>C98/SUM($C$98:$C$101)</f>
+        <v>0.38005202036207025</v>
+      </c>
+      <c r="G98" s="53">
+        <f>C90</f>
+        <v>3566.0227217178694</v>
+      </c>
+      <c r="H98" s="53">
+        <f>C91</f>
+        <v>1116.8385420360898</v>
+      </c>
+      <c r="I98" s="53">
+        <f>C92</f>
+        <v>30.858630944435109</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9">
+      <c r="B99" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-    </row>
-    <row r="3" spans="1:13" ht="31" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="11">
-        <v>277.54000000000002</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="11">
-        <v>363</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16" thickBot="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="16">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="10">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>20146.599999999999</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="22">
-        <v>1E-14</v>
-      </c>
-      <c r="L7" s="10">
-        <v>61266.35</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="11">
-        <v>2.02</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="12">
-        <v>2.8000000000000002E-12</v>
-      </c>
-      <c r="E9" s="11">
-        <v>11415.9</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="12">
-        <v>4.7200000000000001E-12</v>
-      </c>
-      <c r="L9" s="11">
-        <v>9515</v>
-      </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" thickBot="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="K10" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="18">
-        <v>5.77</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="18">
-        <v>7.84</v>
-      </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="13">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="13">
-        <v>69.5</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="11">
-        <v>3.54</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="11">
-        <v>1.73</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.94</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K14" s="11">
-        <v>0.96</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="11">
-        <v>0.02</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="16" thickBot="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21" t="s">
+      <c r="C99" s="64">
+        <f>F88</f>
+        <v>1.8517164822902819E-4</v>
+      </c>
+      <c r="D99" s="64">
+        <f>F89</f>
+        <v>0.47685800769896347</v>
+      </c>
+      <c r="E99" s="53">
+        <f>D99/SUM($D$98:$D$101)</f>
+        <v>0.45830437784354566</v>
+      </c>
+      <c r="F99" s="53">
+        <f>C99/SUM($C$98:$C$101)</f>
+        <v>0.51339874232089977</v>
+      </c>
+      <c r="G99" s="53">
+        <f>F90</f>
+        <v>2575.2214891405251</v>
+      </c>
+      <c r="H99" s="53">
+        <f>F91</f>
+        <v>583.97448169271343</v>
+      </c>
+      <c r="I99" s="53">
+        <f>F92</f>
+        <v>174.18749004773349</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9">
+      <c r="B100" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" s="64">
+        <f>C73/1000*C74/1000*G36/1000000</f>
+        <v>2.1041664571480475E-5</v>
+      </c>
+      <c r="D100" s="64">
+        <f>C36*C100</f>
+        <v>2.7859163892640149E-2</v>
+      </c>
+      <c r="E100" s="53">
+        <f>D100/SUM($D$98:$D$101)</f>
+        <v>2.677521729512013E-2</v>
+      </c>
+      <c r="F100" s="53">
+        <f>C100/SUM($C$98:$C$101)</f>
+        <v>5.8339190856987952E-2</v>
+      </c>
+      <c r="G100" s="53">
+        <f>C36</f>
+        <v>1324</v>
+      </c>
+      <c r="H100" s="53">
+        <f>D36</f>
+        <v>2000</v>
+      </c>
+      <c r="I100" s="53">
+        <f>E36</f>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9">
+      <c r="B101" t="s">
+        <v>167</v>
+      </c>
+      <c r="C101" s="64">
+        <f>C45</f>
+        <v>1.7388304700256E-5</v>
+      </c>
+      <c r="D101" s="64">
+        <f>C46</f>
+        <v>4.6948422690691202E-2</v>
+      </c>
+      <c r="E101" s="53">
+        <f>D101/SUM($D$98:$D$101)</f>
+        <v>4.5121749670976118E-2</v>
+      </c>
+      <c r="F101" s="53">
+        <f>C101/SUM($C$98:$C$101)</f>
+        <v>4.8210046460042094E-2</v>
+      </c>
+      <c r="G101" s="53">
+        <f>C42</f>
+        <v>2700</v>
+      </c>
+      <c r="H101" s="53">
+        <f>C43</f>
+        <v>870</v>
+      </c>
+      <c r="I101" s="53">
+        <f>C44</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" ht="16" thickBot="1">
+      <c r="E102" s="70"/>
+    </row>
+    <row r="103" spans="2:9">
+      <c r="B103" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="72">
+        <f>MAX(C62,F62)/C5</f>
+        <v>62.493806271103281</v>
+      </c>
+      <c r="D103" s="73"/>
+      <c r="E103" s="70"/>
+    </row>
+    <row r="104" spans="2:9">
+      <c r="B104" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="16">
-        <v>6.7540000000000003E-2</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="16" t="s">
+      <c r="C104" s="75">
+        <f>C73*C74/1000/1000</f>
+        <v>0.84166658285921903</v>
+      </c>
+      <c r="D104" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="16">
-        <v>7.2050000000000003E-2</v>
-      </c>
-      <c r="L16" s="21"/>
-      <c r="M16" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="10">
-        <v>0</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="14"/>
-      <c r="H17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="10">
-        <v>0</v>
-      </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="11">
-        <v>2100</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="E104" s="70"/>
+    </row>
+    <row r="105" spans="2:9">
+      <c r="B105" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="C105" s="75">
+        <f>C64+C75+F64+F75+G36</f>
+        <v>407.85714285714289</v>
+      </c>
+      <c r="D105" s="76" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="30" customHeight="1">
+      <c r="B106" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="C106" s="69">
+        <f>C105*C103/1000</f>
+        <v>25.488545271999985</v>
+      </c>
+      <c r="D106" s="76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" ht="30">
+      <c r="B107" s="80" t="s">
+        <v>209</v>
+      </c>
+      <c r="C107" s="69">
+        <f>C106+2*C41</f>
+        <v>26.488545271999985</v>
+      </c>
+      <c r="D107" s="76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9">
+      <c r="B108" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" s="69">
+        <f>E98*H98+E99*H99+E100*H100+E101*H101</f>
+        <v>885.13366342599079</v>
+      </c>
+      <c r="D108" s="76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9">
+      <c r="B109" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="69">
+        <f>F98*G98+F99*G99+F100*G100+F101*G101</f>
+        <v>2884.7978279051908</v>
+      </c>
+      <c r="D109" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="K19" s="11">
-        <v>2100</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="11">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="11">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="12">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="12">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="16" thickBot="1">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="16">
-        <v>0</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="16">
-        <v>0</v>
-      </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="19"/>
-    </row>
-    <row r="25" spans="1:13" ht="16" thickBot="1">
-      <c r="A25" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="33"/>
-      <c r="H25" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="K25" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" s="31"/>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="27" spans="1:13" ht="20">
-      <c r="A27" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="H27" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="29"/>
-    </row>
-    <row r="28" spans="1:13" ht="31" thickBot="1">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="16" thickBot="1">
-      <c r="A29" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="H29" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="18">
-        <v>20</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K30" s="18">
-        <v>20</v>
-      </c>
-      <c r="L30" s="17"/>
-      <c r="M30" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K31" s="11">
-        <v>0</v>
-      </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" ht="16" thickBot="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32" s="16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L32" s="21"/>
-      <c r="M32" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="20">
-      <c r="A34" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="H34" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="29"/>
-    </row>
-    <row r="35" spans="1:13" ht="31" thickBot="1">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="16" thickBot="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="10">
-        <v>30</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="4"/>
-      <c r="H37" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K37" s="18">
-        <v>52</v>
-      </c>
-      <c r="L37" s="17"/>
-      <c r="M37" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="11">
-        <v>750</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K38" s="11">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" ht="16" thickBot="1">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="13">
-        <v>10</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J39" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="K39" s="16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L39" s="21"/>
-      <c r="M39" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="11">
-        <v>3.676E-3</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="11">
-        <v>1000</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="11">
-        <v>1</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="11">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="16" thickBot="1">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" s="16">
-        <v>2.5</v>
-      </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21" t="s">
-        <v>124</v>
+    </row>
+    <row r="110" spans="2:9" ht="30">
+      <c r="B110" s="80" t="s">
+        <v>212</v>
+      </c>
+      <c r="C110" s="69">
+        <f>E98*I98+E99*I99+E100*I100+E101*I101</f>
+        <v>103.37480593771667</v>
+      </c>
+      <c r="D110" s="76" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="16" thickBot="1">
+      <c r="B111" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="C111" s="78">
+        <f>SUM(D98:D101)</f>
+        <v>1.0404832045085801</v>
+      </c>
+      <c r="D111" s="79" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="H27:M27"/>
+  <mergeCells count="2">
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="E48:F48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$I$4:$I$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>D25 K25</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$H$4:$H$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$G$4:$G$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>F16 M16 F32 M32 F40 M39</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$F$4:$F$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>F11:F12 F20:F21 M11:M12 M20:M21 F30 M37 M30</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$C$4:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>D37</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$B$4:$B$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4 K4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
SPM.py: Updates to make the excel interface a bit cleaner, especially in class cell, Updates to make it work with virtual environment utilities.py: Working towards removing pandas dependency
SPM code looks like it works but still need to do some benchmarking.
</commit_message>
<xml_diff>
--- a/python/parameters.xlsx
+++ b/python/parameters.xlsx
@@ -1,86 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="cycle" sheetId="3" r:id="rId2"/>
-    <sheet name="Lists" sheetId="2" r:id="rId3"/>
-    <sheet name="Cell Properties" sheetId="4" r:id="rId4"/>
+    <sheet name="Cell info" sheetId="5" r:id="rId1"/>
+    <sheet name="parameters" sheetId="1" r:id="rId2"/>
+    <sheet name="Cell Properties" sheetId="4" r:id="rId3"/>
+    <sheet name="cycle" sheetId="3" r:id="rId4"/>
+    <sheet name="Lists" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'Cell Properties'!$I$4:$I$9</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Cell Properties'!$I$4</definedName>
-    <definedName name="solver_lhs10" localSheetId="3" hidden="1">'Cell Properties'!$I$8</definedName>
-    <definedName name="solver_lhs11" localSheetId="3" hidden="1">'Cell Properties'!$I$9</definedName>
-    <definedName name="solver_lhs12" localSheetId="3" hidden="1">'Cell Properties'!$I$9</definedName>
-    <definedName name="solver_lhs13" localSheetId="3" hidden="1">'Cell Properties'!$J$6</definedName>
-    <definedName name="solver_lhs14" localSheetId="3" hidden="1">'Cell Properties'!$J$7</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Cell Properties'!$I$5</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Cell Properties'!$I$5</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
-    <definedName name="solver_lhs6" localSheetId="3" hidden="1">'Cell Properties'!$I$6</definedName>
-    <definedName name="solver_lhs7" localSheetId="3" hidden="1">'Cell Properties'!$I$7</definedName>
-    <definedName name="solver_lhs8" localSheetId="3" hidden="1">'Cell Properties'!$I$7</definedName>
-    <definedName name="solver_lhs9" localSheetId="3" hidden="1">'Cell Properties'!$I$8</definedName>
-    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">14</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'Cell Properties'!$I$12</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel10" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel11" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel12" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel13" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel14" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel7" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel8" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel9" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">10</definedName>
-    <definedName name="solver_rhs10" localSheetId="3" hidden="1">0.85</definedName>
-    <definedName name="solver_rhs11" localSheetId="3" hidden="1">0.98</definedName>
-    <definedName name="solver_rhs12" localSheetId="3" hidden="1">0.9</definedName>
-    <definedName name="solver_rhs13" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rhs14" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">20</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'Cell Properties'!$J$5</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_rhs6" localSheetId="3" hidden="1">20</definedName>
-    <definedName name="solver_rhs7" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rhs8" localSheetId="3" hidden="1">0.5</definedName>
-    <definedName name="solver_rhs9" localSheetId="3" hidden="1">0.98</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Cell Properties'!$I$4:$I$9</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Cell Properties'!$I$4</definedName>
+    <definedName name="solver_lhs10" localSheetId="2" hidden="1">'Cell Properties'!$I$8</definedName>
+    <definedName name="solver_lhs11" localSheetId="2" hidden="1">'Cell Properties'!$I$9</definedName>
+    <definedName name="solver_lhs12" localSheetId="2" hidden="1">'Cell Properties'!$I$9</definedName>
+    <definedName name="solver_lhs13" localSheetId="2" hidden="1">'Cell Properties'!$J$6</definedName>
+    <definedName name="solver_lhs14" localSheetId="2" hidden="1">'Cell Properties'!$J$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Cell Properties'!$I$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Cell Properties'!$I$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Cell Properties'!$I$6</definedName>
+    <definedName name="solver_lhs7" localSheetId="2" hidden="1">'Cell Properties'!$I$7</definedName>
+    <definedName name="solver_lhs8" localSheetId="2" hidden="1">'Cell Properties'!$I$7</definedName>
+    <definedName name="solver_lhs9" localSheetId="2" hidden="1">'Cell Properties'!$I$8</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">14</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Cell Properties'!$I$12</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel13" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel14" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">10</definedName>
+    <definedName name="solver_rhs10" localSheetId="2" hidden="1">0.85</definedName>
+    <definedName name="solver_rhs11" localSheetId="2" hidden="1">0.98</definedName>
+    <definedName name="solver_rhs12" localSheetId="2" hidden="1">0.9</definedName>
+    <definedName name="solver_rhs13" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs14" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">20</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">'Cell Properties'!$J$5</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">20</definedName>
+    <definedName name="solver_rhs7" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs8" localSheetId="2" hidden="1">0.5</definedName>
+    <definedName name="solver_rhs9" localSheetId="2" hidden="1">0.98</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -174,190 +175,6 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Ben Kenney</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-cc = constant current
-cv = constant voltage</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Automatically generated.
-The index number associated with either cc or cv modes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Either the current (A) or the voltage (V) that this step should apply.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The stop condition for the step.
-Ex: Run in cc mode until a [voltage | time | DOD | current] stop condition is met.
-The current stop condition is only valid for cv mode.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Automatically generated.
-This is the index number associated with the stop type. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This is the actual stop condition. 
-Either current (A), DOD (fraction), time (s), voltage (V)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ben Kenney:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The maximum time step size in the simulation of this step. The step will start off with a small dt value and gradually increase until it hits this maximum time step .</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Dana</author>
@@ -643,8 +460,192 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ben Kenney</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cc = constant current
+cv = constant voltage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Automatically generated.
+The index number associated with either cc or cv modes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Either the current (A) or the voltage (V) that this step should apply.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The stop condition for the step.
+Ex: Run in cc mode until a [voltage | time | DOD | current] stop condition is met.
+The current stop condition is only valid for cv mode.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Automatically generated.
+This is the index number associated with the stop type. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the actual stop condition. 
+Either current (A), DOD (fraction), time (s), voltage (V)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Kenney:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The maximum time step size in the simulation of this step. The step will start off with a small dt value and gradually increase until it hits this maximum time step .</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="229">
   <si>
     <t>Positive</t>
   </si>
@@ -1328,6 +1329,9 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>LG2200 18650 cell</t>
   </si>
 </sst>
 </file>
@@ -1933,22 +1937,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1990,12 +1978,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2036,6 +2018,28 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2466,11 +2470,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2489,23 +2518,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="20">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102"/>
       <c r="G2"/>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5"/>
@@ -3155,10 +3184,10 @@
       <c r="C25" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="E25" s="48"/>
+      <c r="E25" s="103"/>
       <c r="F25" s="24"/>
       <c r="H25" s="24" t="s">
         <v>127</v>
@@ -3169,29 +3198,29 @@
       <c r="J25" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="L25" s="48"/>
+      <c r="L25" s="103"/>
       <c r="M25" s="24"/>
     </row>
     <row r="27" spans="1:13" ht="20">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="47"/>
-      <c r="H27" s="45" t="s">
+      <c r="B27" s="101"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="102"/>
+      <c r="H27" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="47"/>
+      <c r="I27" s="101"/>
+      <c r="J27" s="101"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
+      <c r="M27" s="102"/>
     </row>
     <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="5"/>
@@ -3340,22 +3369,22 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="20">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="47"/>
-      <c r="H34" s="45" t="s">
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="102"/>
+      <c r="H34" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="47"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="102"/>
     </row>
     <row r="35" spans="1:13" ht="16" thickBot="1">
       <c r="A35" s="5"/>
@@ -3451,7 +3480,7 @@
       <c r="C38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="105">
+      <c r="D38" s="98">
         <f>'Cell Properties'!C108</f>
         <v>885.13366342599079</v>
       </c>
@@ -3764,12 +3793,1660 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J111"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10">
+      <c r="B1" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="H3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="20">
+      <c r="B4" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4">
+        <v>62.493806271103288</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="92">
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <v>127</v>
+      </c>
+      <c r="E5">
+        <v>145</v>
+      </c>
+      <c r="F5">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5">
+        <v>71.428571428571445</v>
+      </c>
+      <c r="J5">
+        <f>I5*1.4</f>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="92">
+        <v>148</v>
+      </c>
+      <c r="D6">
+        <v>177</v>
+      </c>
+      <c r="E6">
+        <v>192</v>
+      </c>
+      <c r="F6">
+        <v>148</v>
+      </c>
+      <c r="H6" t="s">
+        <v>218</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6" s="51">
+        <f>F20-F19</f>
+        <v>-2.9999999928698173E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="H7" t="s">
+        <v>219</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="51">
+        <f>F29-F28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8">
+        <v>0.88000002999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="47">
+        <f>C107</f>
+        <v>26.488545271999985</v>
+      </c>
+      <c r="D9">
+        <v>26.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="48">
+        <f>C111</f>
+        <v>1.0404832045085801</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="C11" s="49"/>
+      <c r="H11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="96">
+        <f>I4</f>
+        <v>62.493806271103288</v>
+      </c>
+      <c r="H12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I12" s="99">
+        <f>(C9-D9)^2+(C10-D10)^2</f>
+        <v>8.4511702895127896E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="C13" s="96"/>
+      <c r="I13" s="99"/>
+    </row>
+    <row r="14" spans="2:10" ht="20">
+      <c r="B14" s="46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="54">
+        <v>4750</v>
+      </c>
+      <c r="D18" s="92">
+        <v>1172</v>
+      </c>
+      <c r="E18" s="92">
+        <v>5</v>
+      </c>
+      <c r="F18" s="94">
+        <f>I8</f>
+        <v>0.88000002999999993</v>
+      </c>
+      <c r="G18" s="52">
+        <f>(F18/C18)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.74725341099764386</v>
+      </c>
+      <c r="H18" s="52">
+        <f>G18*(1-$C$85)</f>
+        <v>0.65583160130526308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="53">
+        <v>2100</v>
+      </c>
+      <c r="D19" s="92">
+        <v>710</v>
+      </c>
+      <c r="E19" s="92">
+        <v>100</v>
+      </c>
+      <c r="F19" s="94">
+        <f>I10</f>
+        <v>0.06</v>
+      </c>
+      <c r="G19" s="52">
+        <f>(F19/C19)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.11524199939073732</v>
+      </c>
+      <c r="H19" s="52">
+        <f>G19*(1-$C$85)</f>
+        <v>0.10114285714285713</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="54">
+        <v>1760</v>
+      </c>
+      <c r="D20" s="92">
+        <v>2500</v>
+      </c>
+      <c r="E20" s="92">
+        <v>1</v>
+      </c>
+      <c r="F20" s="95">
+        <f>1-F18-F19</f>
+        <v>5.9999970000000069E-2</v>
+      </c>
+      <c r="G20" s="52">
+        <f>(F20/C20)/(F18/C18+F19/C19+F20/C20)</f>
+        <v>0.13750458961161893</v>
+      </c>
+      <c r="H20" s="52">
+        <f>G20*(1-$C$85)</f>
+        <v>0.12068175784090925</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="54">
+        <v>1204</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="52">
+        <f>$C$85</f>
+        <v>0.12234378371097065</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="C22" s="55"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="56"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="C23" s="55"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="56"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" t="s">
+        <v>155</v>
+      </c>
+      <c r="H25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="54">
+        <v>2100</v>
+      </c>
+      <c r="D27" s="92">
+        <v>710</v>
+      </c>
+      <c r="E27" s="92">
+        <v>100</v>
+      </c>
+      <c r="F27" s="94">
+        <f>I9</f>
+        <v>0.9</v>
+      </c>
+      <c r="G27" s="52">
+        <f>(F27/C27)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>0.89138998311761397</v>
+      </c>
+      <c r="H27" s="52">
+        <f>G27*(1-$F$85)</f>
+        <v>0.74142857142857155</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="53">
+        <v>2100</v>
+      </c>
+      <c r="D28" s="92">
+        <v>710</v>
+      </c>
+      <c r="E28" s="92">
+        <v>100</v>
+      </c>
+      <c r="F28" s="94">
+        <v>0.05</v>
+      </c>
+      <c r="G28" s="52">
+        <f>(F28/C28)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>4.9521665728756332E-2</v>
+      </c>
+      <c r="H28" s="52">
+        <f>G28*(1-$F$85)</f>
+        <v>4.1190476190476194E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="54">
+        <v>1760</v>
+      </c>
+      <c r="D29" s="92">
+        <v>2500</v>
+      </c>
+      <c r="E29" s="92">
+        <v>1</v>
+      </c>
+      <c r="F29" s="95">
+        <f>1-F27-F28</f>
+        <v>4.9999999999999975E-2</v>
+      </c>
+      <c r="G29" s="52">
+        <f>(F29/C29)/(F27/C27+F28/C28+F29/C29)</f>
+        <v>5.9088351153629683E-2</v>
+      </c>
+      <c r="H29" s="52">
+        <f>G29*(1-$F$85)</f>
+        <v>4.9147727272727253E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="54">
+        <v>1204</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52">
+        <f>$F$85</f>
+        <v>0.16823322510822503</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" s="55"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+    </row>
+    <row r="33" spans="2:8" ht="20">
+      <c r="B33" s="46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="20">
+      <c r="B34" s="46"/>
+      <c r="C34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="92">
+        <v>1324</v>
+      </c>
+      <c r="D36" s="92">
+        <v>2000</v>
+      </c>
+      <c r="E36" s="92">
+        <v>0.83</v>
+      </c>
+      <c r="F36" s="93">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G36" s="92">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="45"/>
+      <c r="F37" s="57"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="45"/>
+      <c r="F38" s="57"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="57"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" t="s">
+        <v>215</v>
+      </c>
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" s="57"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="92">
+        <f>I7</f>
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="92">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="57"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" s="91">
+        <v>2700</v>
+      </c>
+      <c r="D42" s="92">
+        <v>1150</v>
+      </c>
+      <c r="F42" s="57"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="91">
+        <v>870</v>
+      </c>
+      <c r="D43" s="92">
+        <v>1900</v>
+      </c>
+      <c r="F43" s="57"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="91">
+        <v>200</v>
+      </c>
+      <c r="D44" s="92">
+        <v>0.16</v>
+      </c>
+      <c r="F44" s="57"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="59">
+        <f>(C5/1000*C6/1000*2+C6/1000*C9/1000*2)*C41/1000</f>
+        <v>1.7388304700256E-5</v>
+      </c>
+      <c r="D45" s="92"/>
+      <c r="F45" s="57"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="59">
+        <f>C42*C45</f>
+        <v>4.6948422690691202E-2</v>
+      </c>
+      <c r="D46" s="92"/>
+      <c r="F46" s="57"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="105" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="106"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="105" t="s">
+        <v>176</v>
+      </c>
+      <c r="F48" s="106"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="77"/>
+      <c r="E49" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="77"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="77" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="90">
+        <v>10</v>
+      </c>
+      <c r="E51" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="F51" s="90">
+        <v>10</v>
+      </c>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="90">
+        <v>25</v>
+      </c>
+      <c r="E52" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="90">
+        <v>25</v>
+      </c>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="90">
+        <v>20</v>
+      </c>
+      <c r="D53" s="62"/>
+      <c r="E53" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="90">
+        <v>20</v>
+      </c>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="91">
+        <v>2700</v>
+      </c>
+      <c r="E54" s="80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F54" s="91">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" s="91">
+        <v>870</v>
+      </c>
+      <c r="E55" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="F55" s="91">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="91">
+        <v>200</v>
+      </c>
+      <c r="E56" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="90">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="82">
+        <f>C51/1000*C52/1000*C53/1000000</f>
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="E57" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" s="82">
+        <f>F51/1000*F52/1000*F53/1000000</f>
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="C58" s="82">
+        <f>C57*C54</f>
+        <v>1.3499999999999999E-5</v>
+      </c>
+      <c r="E58" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" s="82">
+        <f>F57*F54</f>
+        <v>4.5000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="80"/>
+      <c r="C59" s="81"/>
+      <c r="E59" s="80"/>
+      <c r="F59" s="81"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="77"/>
+      <c r="E60" s="76" t="s">
+        <v>183</v>
+      </c>
+      <c r="F60" s="77"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="77" t="s">
+        <v>178</v>
+      </c>
+      <c r="E61" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="77" t="s">
+        <v>179</v>
+      </c>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="97">
+        <f>C5*C12</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="E62" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="97">
+        <f>C5*C12</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="97">
+        <f>C6</f>
+        <v>148</v>
+      </c>
+      <c r="E63" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="97">
+        <f>C6</f>
+        <v>148</v>
+      </c>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="91">
+        <v>20</v>
+      </c>
+      <c r="E64" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="F64" s="91">
+        <v>20</v>
+      </c>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="90">
+        <v>2700</v>
+      </c>
+      <c r="E65" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="F65" s="91">
+        <v>9000</v>
+      </c>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="91">
+        <v>870</v>
+      </c>
+      <c r="E66" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="F66" s="91">
+        <v>381</v>
+      </c>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="91">
+        <v>200</v>
+      </c>
+      <c r="E67" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="F67" s="90">
+        <v>380</v>
+      </c>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" s="82">
+        <f>C62/1000*C63/1000*C64/1000000</f>
+        <v>1.6833331657184382E-5</v>
+      </c>
+      <c r="E68" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="F68" s="82">
+        <f>F62/1000*F63/1000*F64/1000000</f>
+        <v>1.6833331657184382E-5</v>
+      </c>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" s="82">
+        <f>C68*C65</f>
+        <v>4.5449995474397833E-2</v>
+      </c>
+      <c r="E69" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="F69" s="82">
+        <f>F68*F65</f>
+        <v>0.15149998491465944</v>
+      </c>
+      <c r="G69" s="62"/>
+      <c r="H69" s="62"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="80"/>
+      <c r="C70" s="81"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="81"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="77"/>
+      <c r="E71" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="F71" s="77"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+    </row>
+    <row r="72" spans="2:8" ht="30">
+      <c r="B72" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="F72" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="97">
+        <f>C62</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="E73" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="F73" s="97">
+        <f>F62</f>
+        <v>5686.9363706703989</v>
+      </c>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="97">
+        <f>C63</f>
+        <v>148</v>
+      </c>
+      <c r="E74" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="F74" s="97">
+        <f>F63</f>
+        <v>148</v>
+      </c>
+      <c r="G74" s="62"/>
+      <c r="H74" s="62"/>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="B75" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" s="91">
+        <f>2*I5</f>
+        <v>142.85714285714289</v>
+      </c>
+      <c r="E75" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="F75" s="91">
+        <f>2*I6</f>
+        <v>200</v>
+      </c>
+      <c r="G75" s="63"/>
+      <c r="H75" s="63"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="83">
+        <f>(C18*H18+H19*C19+C20*H20+C21*H21)</f>
+        <v>3687.3019155880088</v>
+      </c>
+      <c r="E76" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="F76" s="83">
+        <f>(H27*C27+C28*H28+H29*C29+H30*C30)</f>
+        <v>1932.552803030303</v>
+      </c>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63"/>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="B77" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="82">
+        <f>C73/1000*C74/1000*C75/1000000</f>
+        <v>1.2023808326560274E-4</v>
+      </c>
+      <c r="E77" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="F77" s="82">
+        <f>F73/1000*F74/1000*F75/1000000</f>
+        <v>1.683333165718438E-4</v>
+      </c>
+      <c r="G77" s="63"/>
+      <c r="H77" s="63"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="C78" s="82">
+        <f>C77*C76</f>
+        <v>0.44335411475188752</v>
+      </c>
+      <c r="E78" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="F78" s="82">
+        <f>F77*F76</f>
+        <v>0.32531302278430407</v>
+      </c>
+      <c r="G78" s="63"/>
+      <c r="H78" s="63"/>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="83">
+        <f>D18*H18+D19*H19+D20*H20</f>
+        <v>1142.1504599034699</v>
+      </c>
+      <c r="E79" s="80" t="s">
+        <v>68</v>
+      </c>
+      <c r="F79" s="83">
+        <f>H27*D27+H28*D28+H29*D29</f>
+        <v>678.52884199134201</v>
+      </c>
+      <c r="G79" s="63"/>
+      <c r="H79" s="63"/>
+    </row>
+    <row r="80" spans="2:8">
+      <c r="B80" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="83">
+        <f>E18*H18+E19*H19+E20*H20</f>
+        <v>13.514125478652939</v>
+      </c>
+      <c r="E80" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="F80" s="83">
+        <f>H27*E27+H28*E28+H29*E29</f>
+        <v>78.311052489177499</v>
+      </c>
+      <c r="G80" s="63"/>
+      <c r="H80" s="63"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="80"/>
+      <c r="C81" s="81"/>
+      <c r="E81" s="80"/>
+      <c r="F81" s="81"/>
+      <c r="G81" s="63"/>
+      <c r="H81" s="63"/>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" s="84" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="77"/>
+      <c r="E82" s="84" t="s">
+        <v>189</v>
+      </c>
+      <c r="F82" s="77"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" s="90">
+        <f>parameters!D13</f>
+        <v>3.54</v>
+      </c>
+      <c r="E83" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="90">
+        <f>parameters!K13</f>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="B84" s="80" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="83">
+        <f>(C18*G18+C19*G19+C20*G20)/1000</f>
+        <v>4.0334699786758064</v>
+      </c>
+      <c r="E84" s="80" t="s">
+        <v>191</v>
+      </c>
+      <c r="F84" s="83">
+        <f>(C27*G27+C28*G28+C29*G29)/1000</f>
+        <v>2.0799099606077656</v>
+      </c>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="B85" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="85">
+        <f>1-C83/C84</f>
+        <v>0.12234378371097065</v>
+      </c>
+      <c r="E85" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85" s="85">
+        <f>1-F83/F84</f>
+        <v>0.16823322510822503</v>
+      </c>
+      <c r="G85" s="51"/>
+      <c r="H85" s="51"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="80"/>
+      <c r="C86" s="86"/>
+      <c r="E86" s="80"/>
+      <c r="F86" s="86"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="51"/>
+    </row>
+    <row r="87" spans="2:9">
+      <c r="B87" s="84" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" s="77"/>
+      <c r="E87" s="84" t="s">
+        <v>192</v>
+      </c>
+      <c r="F87" s="77"/>
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="82">
+        <f>C57+C68+C77</f>
+        <v>1.3707641492278713E-4</v>
+      </c>
+      <c r="E88" s="79" t="s">
+        <v>193</v>
+      </c>
+      <c r="F88" s="82">
+        <f>F57+F68+F77</f>
+        <v>1.8517164822902819E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9">
+      <c r="B89" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" s="82">
+        <f>C58+C69+C78</f>
+        <v>0.48881761022628534</v>
+      </c>
+      <c r="E89" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="F89" s="82">
+        <f>F58+F69+F78</f>
+        <v>0.47685800769896347</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9">
+      <c r="B90" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" s="83">
+        <f>C89/C88</f>
+        <v>3566.0227217178694</v>
+      </c>
+      <c r="E90" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="F90" s="83">
+        <f>F89/F88</f>
+        <v>2575.2214891405251</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="B91" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="C91" s="83">
+        <f>C79*(C78/$C$89)+C66*(C69/$C$89)+C55*(C58/$C$89)</f>
+        <v>1116.8385420360898</v>
+      </c>
+      <c r="E91" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="F91" s="83">
+        <f>F79*(F78/$F$89)+F66*(F69/$F$89)+F55*(F58/$F$89)</f>
+        <v>583.97448169271343</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9">
+      <c r="B92" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" s="88">
+        <f>C80*(C78/$C$89)+C67*(C69/$C$89)+C56*(C58/$C$89)</f>
+        <v>30.858630944435109</v>
+      </c>
+      <c r="E92" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="F92" s="88">
+        <f>F80*(F78/$F$89)+F67*(F69/$F$89)+F56*(F58/$F$89)</f>
+        <v>174.18749004773349</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="B95" s="45" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="C96" t="s">
+        <v>199</v>
+      </c>
+      <c r="D96" t="s">
+        <v>200</v>
+      </c>
+      <c r="E96" t="s">
+        <v>201</v>
+      </c>
+      <c r="F96" t="s">
+        <v>202</v>
+      </c>
+      <c r="G96" t="s">
+        <v>42</v>
+      </c>
+      <c r="H96" t="s">
+        <v>68</v>
+      </c>
+      <c r="I96" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9">
+      <c r="C97" t="s">
+        <v>203</v>
+      </c>
+      <c r="D97" t="s">
+        <v>204</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+      <c r="F97" t="s">
+        <v>135</v>
+      </c>
+      <c r="G97" t="s">
+        <v>36</v>
+      </c>
+      <c r="H97" t="s">
+        <v>73</v>
+      </c>
+      <c r="I97" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9">
+      <c r="B98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="59">
+        <f>C88</f>
+        <v>1.3707641492278713E-4</v>
+      </c>
+      <c r="D98" s="59">
+        <f>C89</f>
+        <v>0.48881761022628534</v>
+      </c>
+      <c r="E98" s="48">
+        <f>D98/SUM($D$98:$D$101)</f>
+        <v>0.46979865519035813</v>
+      </c>
+      <c r="F98" s="48">
+        <f>C98/SUM($C$98:$C$101)</f>
+        <v>0.38005202036207025</v>
+      </c>
+      <c r="G98" s="48">
+        <f>C90</f>
+        <v>3566.0227217178694</v>
+      </c>
+      <c r="H98" s="48">
+        <f>C91</f>
+        <v>1116.8385420360898</v>
+      </c>
+      <c r="I98" s="48">
+        <f>C92</f>
+        <v>30.858630944435109</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9">
+      <c r="B99" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" s="59">
+        <f>F88</f>
+        <v>1.8517164822902819E-4</v>
+      </c>
+      <c r="D99" s="59">
+        <f>F89</f>
+        <v>0.47685800769896347</v>
+      </c>
+      <c r="E99" s="48">
+        <f>D99/SUM($D$98:$D$101)</f>
+        <v>0.45830437784354566</v>
+      </c>
+      <c r="F99" s="48">
+        <f>C99/SUM($C$98:$C$101)</f>
+        <v>0.51339874232089977</v>
+      </c>
+      <c r="G99" s="48">
+        <f>F90</f>
+        <v>2575.2214891405251</v>
+      </c>
+      <c r="H99" s="48">
+        <f>F91</f>
+        <v>583.97448169271343</v>
+      </c>
+      <c r="I99" s="48">
+        <f>F92</f>
+        <v>174.18749004773349</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9">
+      <c r="B100" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" s="59">
+        <f>C73/1000*C74/1000*G36/1000000</f>
+        <v>2.1041664571480475E-5</v>
+      </c>
+      <c r="D100" s="59">
+        <f>C36*C100</f>
+        <v>2.7859163892640149E-2</v>
+      </c>
+      <c r="E100" s="48">
+        <f>D100/SUM($D$98:$D$101)</f>
+        <v>2.677521729512013E-2</v>
+      </c>
+      <c r="F100" s="48">
+        <f>C100/SUM($C$98:$C$101)</f>
+        <v>5.8339190856987952E-2</v>
+      </c>
+      <c r="G100" s="48">
+        <f>C36</f>
+        <v>1324</v>
+      </c>
+      <c r="H100" s="48">
+        <f>D36</f>
+        <v>2000</v>
+      </c>
+      <c r="I100" s="48">
+        <f>E36</f>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9">
+      <c r="B101" t="s">
+        <v>167</v>
+      </c>
+      <c r="C101" s="59">
+        <f>C45</f>
+        <v>1.7388304700256E-5</v>
+      </c>
+      <c r="D101" s="59">
+        <f>C46</f>
+        <v>4.6948422690691202E-2</v>
+      </c>
+      <c r="E101" s="48">
+        <f>D101/SUM($D$98:$D$101)</f>
+        <v>4.5121749670976118E-2</v>
+      </c>
+      <c r="F101" s="48">
+        <f>C101/SUM($C$98:$C$101)</f>
+        <v>4.8210046460042094E-2</v>
+      </c>
+      <c r="G101" s="48">
+        <f>C42</f>
+        <v>2700</v>
+      </c>
+      <c r="H101" s="48">
+        <f>C43</f>
+        <v>870</v>
+      </c>
+      <c r="I101" s="48">
+        <f>C44</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" ht="16" thickBot="1">
+      <c r="E102" s="65"/>
+    </row>
+    <row r="103" spans="2:9">
+      <c r="B103" s="66" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="67">
+        <f>MAX(C62,F62)/C5</f>
+        <v>62.493806271103281</v>
+      </c>
+      <c r="D103" s="68"/>
+      <c r="E103" s="65"/>
+    </row>
+    <row r="104" spans="2:9">
+      <c r="B104" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" s="70">
+        <f>C73*C74/1000/1000</f>
+        <v>0.84166658285921903</v>
+      </c>
+      <c r="D104" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="65"/>
+    </row>
+    <row r="105" spans="2:9">
+      <c r="B105" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="C105" s="70">
+        <f>C64+C75+F64+F75+G36</f>
+        <v>407.85714285714289</v>
+      </c>
+      <c r="D105" s="71" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="30" customHeight="1">
+      <c r="B106" s="75" t="s">
+        <v>208</v>
+      </c>
+      <c r="C106" s="64">
+        <f>C105*C103/1000</f>
+        <v>25.488545271999985</v>
+      </c>
+      <c r="D106" s="71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" ht="30">
+      <c r="B107" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="C107" s="64">
+        <f>C106+2*C41</f>
+        <v>26.488545271999985</v>
+      </c>
+      <c r="D107" s="71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9">
+      <c r="B108" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" s="64">
+        <f>E98*H98+E99*H99+E100*H100+E101*H101</f>
+        <v>885.13366342599079</v>
+      </c>
+      <c r="D108" s="71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9">
+      <c r="B109" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="64">
+        <f>F98*G98+F99*G99+F100*G100+F101*G101</f>
+        <v>2884.7978279051908</v>
+      </c>
+      <c r="D109" s="71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" ht="30">
+      <c r="B110" s="75" t="s">
+        <v>212</v>
+      </c>
+      <c r="C110" s="64">
+        <f>E98*I98+E99*I99+E100*I100+E101*I101</f>
+        <v>103.37480593771667</v>
+      </c>
+      <c r="D110" s="71" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="16" thickBot="1">
+      <c r="B111" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="C111" s="73">
+        <f>SUM(D98:D101)</f>
+        <v>1.0404832045085801</v>
+      </c>
+      <c r="D111" s="74" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="E48:F48"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3787,18 +5464,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="33" t="s">
@@ -4043,7 +5720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L9"/>
   <sheetViews>
@@ -4223,1652 +5900,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J111"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10">
-      <c r="B1" s="50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="H3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="20">
-      <c r="B4" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H4" t="s">
-        <v>216</v>
-      </c>
-      <c r="I4">
-        <v>62.493806271103288</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="99">
-        <v>91</v>
-      </c>
-      <c r="D5">
-        <v>127</v>
-      </c>
-      <c r="E5">
-        <v>145</v>
-      </c>
-      <c r="F5">
-        <v>91</v>
-      </c>
-      <c r="H5" t="s">
-        <v>217</v>
-      </c>
-      <c r="I5">
-        <v>71.428571428571445</v>
-      </c>
-      <c r="J5">
-        <f>I5*1.4</f>
-        <v>100.00000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="99">
-        <v>148</v>
-      </c>
-      <c r="D6">
-        <v>177</v>
-      </c>
-      <c r="E6">
-        <v>192</v>
-      </c>
-      <c r="F6">
-        <v>148</v>
-      </c>
-      <c r="H6" t="s">
-        <v>218</v>
-      </c>
-      <c r="I6">
-        <v>100</v>
-      </c>
-      <c r="J6" s="56">
-        <f>F20-F19</f>
-        <v>-2.9999999928698173E-8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="H7" t="s">
-        <v>219</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7" s="56">
-        <f>F29-F28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="C8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8">
-        <v>0.88000002999999993</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="52">
-        <f>C107</f>
-        <v>26.488545271999985</v>
-      </c>
-      <c r="D9">
-        <v>26.5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>222</v>
-      </c>
-      <c r="I9">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="53">
-        <f>C111</f>
-        <v>1.0404832045085801</v>
-      </c>
-      <c r="D10">
-        <v>0.75</v>
-      </c>
-      <c r="H10" t="s">
-        <v>224</v>
-      </c>
-      <c r="I10">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="C11" s="54"/>
-      <c r="H11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I11">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" s="103">
-        <f>I4</f>
-        <v>62.493806271103288</v>
-      </c>
-      <c r="H12" t="s">
-        <v>223</v>
-      </c>
-      <c r="I12" s="106">
-        <f>(C9-D9)^2+(C10-D10)^2</f>
-        <v>8.4511702895127896E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="C13" s="103"/>
-      <c r="I13" s="106"/>
-    </row>
-    <row r="14" spans="2:10" ht="20">
-      <c r="B14" s="51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="C16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>153</v>
-      </c>
-      <c r="F16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G16" t="s">
-        <v>155</v>
-      </c>
-      <c r="H16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" t="s">
-        <v>157</v>
-      </c>
-      <c r="G17" t="s">
-        <v>157</v>
-      </c>
-      <c r="H17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="59">
-        <v>4750</v>
-      </c>
-      <c r="D18" s="99">
-        <v>1172</v>
-      </c>
-      <c r="E18" s="99">
-        <v>5</v>
-      </c>
-      <c r="F18" s="101">
-        <f>I8</f>
-        <v>0.88000002999999993</v>
-      </c>
-      <c r="G18" s="57">
-        <f>(F18/C18)/(F18/C18+F19/C19+F20/C20)</f>
-        <v>0.74725341099764386</v>
-      </c>
-      <c r="H18" s="57">
-        <f>G18*(1-$C$85)</f>
-        <v>0.65583160130526308</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" s="58">
-        <v>2100</v>
-      </c>
-      <c r="D19" s="99">
-        <v>710</v>
-      </c>
-      <c r="E19" s="99">
-        <v>100</v>
-      </c>
-      <c r="F19" s="101">
-        <f>I10</f>
-        <v>0.06</v>
-      </c>
-      <c r="G19" s="57">
-        <f>(F19/C19)/(F18/C18+F19/C19+F20/C20)</f>
-        <v>0.11524199939073732</v>
-      </c>
-      <c r="H19" s="57">
-        <f>G19*(1-$C$85)</f>
-        <v>0.10114285714285713</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20" s="59">
-        <v>1760</v>
-      </c>
-      <c r="D20" s="99">
-        <v>2500</v>
-      </c>
-      <c r="E20" s="99">
-        <v>1</v>
-      </c>
-      <c r="F20" s="102">
-        <f>1-F18-F19</f>
-        <v>5.9999970000000069E-2</v>
-      </c>
-      <c r="G20" s="57">
-        <f>(F20/C20)/(F18/C18+F19/C19+F20/C20)</f>
-        <v>0.13750458961161893</v>
-      </c>
-      <c r="H20" s="57">
-        <f>G20*(1-$C$85)</f>
-        <v>0.12068175784090925</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="59">
-        <v>1204</v>
-      </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="57">
-        <f>$C$85</f>
-        <v>0.12234378371097065</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="C22" s="60"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="61"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="C23" s="60"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="61"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="C25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" t="s">
-        <v>154</v>
-      </c>
-      <c r="G25" t="s">
-        <v>155</v>
-      </c>
-      <c r="H25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>156</v>
-      </c>
-      <c r="F26" t="s">
-        <v>157</v>
-      </c>
-      <c r="G26" t="s">
-        <v>157</v>
-      </c>
-      <c r="H26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="59">
-        <v>2100</v>
-      </c>
-      <c r="D27" s="99">
-        <v>710</v>
-      </c>
-      <c r="E27" s="99">
-        <v>100</v>
-      </c>
-      <c r="F27" s="101">
-        <f>I9</f>
-        <v>0.9</v>
-      </c>
-      <c r="G27" s="57">
-        <f>(F27/C27)/(F27/C27+F28/C28+F29/C29)</f>
-        <v>0.89138998311761397</v>
-      </c>
-      <c r="H27" s="57">
-        <f>G27*(1-$F$85)</f>
-        <v>0.74142857142857155</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" t="s">
-        <v>159</v>
-      </c>
-      <c r="C28" s="58">
-        <v>2100</v>
-      </c>
-      <c r="D28" s="99">
-        <v>710</v>
-      </c>
-      <c r="E28" s="99">
-        <v>100</v>
-      </c>
-      <c r="F28" s="101">
-        <v>0.05</v>
-      </c>
-      <c r="G28" s="57">
-        <f>(F28/C28)/(F27/C27+F28/C28+F29/C29)</f>
-        <v>4.9521665728756332E-2</v>
-      </c>
-      <c r="H28" s="57">
-        <f>G28*(1-$F$85)</f>
-        <v>4.1190476190476194E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
-      <c r="B29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="59">
-        <v>1760</v>
-      </c>
-      <c r="D29" s="99">
-        <v>2500</v>
-      </c>
-      <c r="E29" s="99">
-        <v>1</v>
-      </c>
-      <c r="F29" s="102">
-        <f>1-F27-F28</f>
-        <v>4.9999999999999975E-2</v>
-      </c>
-      <c r="G29" s="57">
-        <f>(F29/C29)/(F27/C27+F28/C28+F29/C29)</f>
-        <v>5.9088351153629683E-2</v>
-      </c>
-      <c r="H29" s="57">
-        <f>G29*(1-$F$85)</f>
-        <v>4.9147727272727253E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
-        <v>161</v>
-      </c>
-      <c r="C30" s="59">
-        <v>1204</v>
-      </c>
-      <c r="D30" s="60"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57">
-        <f>$F$85</f>
-        <v>0.16823322510822503</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="C31" s="60"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-    </row>
-    <row r="33" spans="2:8" ht="20">
-      <c r="B33" s="51" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="20">
-      <c r="B34" s="51"/>
-      <c r="C34" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="99">
-        <v>1324</v>
-      </c>
-      <c r="D36" s="99">
-        <v>2000</v>
-      </c>
-      <c r="E36" s="99">
-        <v>0.83</v>
-      </c>
-      <c r="F36" s="100">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G36" s="99">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="50"/>
-      <c r="F37" s="62"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="50"/>
-      <c r="F38" s="62"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="F39" s="62"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="63" t="s">
-        <v>168</v>
-      </c>
-      <c r="C40" t="s">
-        <v>215</v>
-      </c>
-      <c r="D40" t="s">
-        <v>169</v>
-      </c>
-      <c r="F40" s="62"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" s="99">
-        <f>I7</f>
-        <v>0.5</v>
-      </c>
-      <c r="D41" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="F41" s="62"/>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="63" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="98">
-        <v>2700</v>
-      </c>
-      <c r="D42" s="99">
-        <v>1150</v>
-      </c>
-      <c r="F42" s="62"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="98">
-        <v>870</v>
-      </c>
-      <c r="D43" s="99">
-        <v>1900</v>
-      </c>
-      <c r="F43" s="62"/>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="63" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" s="98">
-        <v>200</v>
-      </c>
-      <c r="D44" s="99">
-        <v>0.16</v>
-      </c>
-      <c r="F44" s="62"/>
-    </row>
-    <row r="45" spans="2:8">
-      <c r="B45" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" s="64">
-        <f>(C5/1000*C6/1000*2+C6/1000*C9/1000*2)*C41/1000</f>
-        <v>1.7388304700256E-5</v>
-      </c>
-      <c r="D45" s="99"/>
-      <c r="F45" s="62"/>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="64">
-        <f>C42*C45</f>
-        <v>4.6948422690691202E-2</v>
-      </c>
-      <c r="D46" s="99"/>
-      <c r="F46" s="62"/>
-    </row>
-    <row r="48" spans="2:8">
-      <c r="B48" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="65"/>
-      <c r="E48" s="81" t="s">
-        <v>176</v>
-      </c>
-      <c r="F48" s="82"/>
-      <c r="G48" s="66"/>
-      <c r="H48" s="66"/>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" s="83" t="s">
-        <v>177</v>
-      </c>
-      <c r="C49" s="84"/>
-      <c r="E49" s="83" t="s">
-        <v>177</v>
-      </c>
-      <c r="F49" s="84"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="67"/>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="C50" s="84" t="s">
-        <v>178</v>
-      </c>
-      <c r="E50" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="F50" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="97">
-        <v>10</v>
-      </c>
-      <c r="E51" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="97">
-        <v>10</v>
-      </c>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="97">
-        <v>25</v>
-      </c>
-      <c r="E52" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="F52" s="97">
-        <v>25</v>
-      </c>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="97">
-        <v>20</v>
-      </c>
-      <c r="D53" s="67"/>
-      <c r="E53" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="F53" s="97">
-        <v>20</v>
-      </c>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-    </row>
-    <row r="54" spans="2:8">
-      <c r="B54" s="87" t="s">
-        <v>170</v>
-      </c>
-      <c r="C54" s="98">
-        <v>2700</v>
-      </c>
-      <c r="E54" s="87" t="s">
-        <v>170</v>
-      </c>
-      <c r="F54" s="98">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="87" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="98">
-        <v>870</v>
-      </c>
-      <c r="E55" s="87" t="s">
-        <v>181</v>
-      </c>
-      <c r="F55" s="98">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="98">
-        <v>200</v>
-      </c>
-      <c r="E56" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="F56" s="97">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="C57" s="89">
-        <f>C51/1000*C52/1000*C53/1000000</f>
-        <v>5.0000000000000001E-9</v>
-      </c>
-      <c r="E57" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="F57" s="89">
-        <f>F51/1000*F52/1000*F53/1000000</f>
-        <v>5.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="C58" s="89">
-        <f>C57*C54</f>
-        <v>1.3499999999999999E-5</v>
-      </c>
-      <c r="E58" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="F58" s="89">
-        <f>F57*F54</f>
-        <v>4.5000000000000003E-5</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="87"/>
-      <c r="C59" s="88"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="88"/>
-    </row>
-    <row r="60" spans="2:8">
-      <c r="B60" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="C60" s="84"/>
-      <c r="E60" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="F60" s="84"/>
-      <c r="G60" s="67"/>
-      <c r="H60" s="67"/>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="C61" s="84" t="s">
-        <v>178</v>
-      </c>
-      <c r="E61" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="F61" s="84" t="s">
-        <v>179</v>
-      </c>
-      <c r="G61" s="67"/>
-      <c r="H61" s="67"/>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="104">
-        <f>C5*C12</f>
-        <v>5686.9363706703989</v>
-      </c>
-      <c r="E62" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="F62" s="104">
-        <f>C5*C12</f>
-        <v>5686.9363706703989</v>
-      </c>
-      <c r="G62" s="67"/>
-      <c r="H62" s="67"/>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="104">
-        <f>C6</f>
-        <v>148</v>
-      </c>
-      <c r="E63" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="F63" s="104">
-        <f>C6</f>
-        <v>148</v>
-      </c>
-      <c r="G63" s="67"/>
-      <c r="H63" s="67"/>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="87" t="s">
-        <v>184</v>
-      </c>
-      <c r="C64" s="98">
-        <v>20</v>
-      </c>
-      <c r="E64" s="87" t="s">
-        <v>184</v>
-      </c>
-      <c r="F64" s="98">
-        <v>20</v>
-      </c>
-      <c r="G64" s="67"/>
-      <c r="H64" s="67"/>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" s="87" t="s">
-        <v>185</v>
-      </c>
-      <c r="C65" s="97">
-        <v>2700</v>
-      </c>
-      <c r="E65" s="87" t="s">
-        <v>185</v>
-      </c>
-      <c r="F65" s="98">
-        <v>9000</v>
-      </c>
-      <c r="G65" s="67"/>
-      <c r="H65" s="67"/>
-    </row>
-    <row r="66" spans="2:8">
-      <c r="B66" s="87" t="s">
-        <v>181</v>
-      </c>
-      <c r="C66" s="98">
-        <v>870</v>
-      </c>
-      <c r="E66" s="87" t="s">
-        <v>181</v>
-      </c>
-      <c r="F66" s="98">
-        <v>381</v>
-      </c>
-      <c r="G66" s="67"/>
-      <c r="H66" s="67"/>
-    </row>
-    <row r="67" spans="2:8">
-      <c r="B67" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="C67" s="98">
-        <v>200</v>
-      </c>
-      <c r="E67" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="F67" s="97">
-        <v>380</v>
-      </c>
-      <c r="G67" s="67"/>
-      <c r="H67" s="67"/>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="C68" s="89">
-        <f>C62/1000*C63/1000*C64/1000000</f>
-        <v>1.6833331657184382E-5</v>
-      </c>
-      <c r="E68" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="F68" s="89">
-        <f>F62/1000*F63/1000*F64/1000000</f>
-        <v>1.6833331657184382E-5</v>
-      </c>
-      <c r="G68" s="67"/>
-      <c r="H68" s="67"/>
-    </row>
-    <row r="69" spans="2:8">
-      <c r="B69" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="C69" s="89">
-        <f>C68*C65</f>
-        <v>4.5449995474397833E-2</v>
-      </c>
-      <c r="E69" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="F69" s="89">
-        <f>F68*F65</f>
-        <v>0.15149998491465944</v>
-      </c>
-      <c r="G69" s="67"/>
-      <c r="H69" s="67"/>
-    </row>
-    <row r="70" spans="2:8">
-      <c r="B70" s="87"/>
-      <c r="C70" s="88"/>
-      <c r="E70" s="87"/>
-      <c r="F70" s="88"/>
-      <c r="G70" s="67"/>
-      <c r="H70" s="67"/>
-    </row>
-    <row r="71" spans="2:8">
-      <c r="B71" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="C71" s="84"/>
-      <c r="E71" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="F71" s="84"/>
-      <c r="G71" s="67"/>
-      <c r="H71" s="67"/>
-    </row>
-    <row r="72" spans="2:8" ht="30">
-      <c r="B72" s="85" t="s">
-        <v>187</v>
-      </c>
-      <c r="C72" s="96" t="s">
-        <v>188</v>
-      </c>
-      <c r="E72" s="85" t="s">
-        <v>187</v>
-      </c>
-      <c r="F72" s="96" t="s">
-        <v>188</v>
-      </c>
-      <c r="G72" s="67"/>
-      <c r="H72" s="67"/>
-    </row>
-    <row r="73" spans="2:8">
-      <c r="B73" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="C73" s="104">
-        <f>C62</f>
-        <v>5686.9363706703989</v>
-      </c>
-      <c r="E73" s="86" t="s">
-        <v>145</v>
-      </c>
-      <c r="F73" s="104">
-        <f>F62</f>
-        <v>5686.9363706703989</v>
-      </c>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
-    </row>
-    <row r="74" spans="2:8">
-      <c r="B74" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74" s="104">
-        <f>C63</f>
-        <v>148</v>
-      </c>
-      <c r="E74" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="F74" s="104">
-        <f>F63</f>
-        <v>148</v>
-      </c>
-      <c r="G74" s="67"/>
-      <c r="H74" s="67"/>
-    </row>
-    <row r="75" spans="2:8">
-      <c r="B75" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="C75" s="98">
-        <f>2*I5</f>
-        <v>142.85714285714289</v>
-      </c>
-      <c r="E75" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="F75" s="98">
-        <f>2*I6</f>
-        <v>200</v>
-      </c>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
-    </row>
-    <row r="76" spans="2:8">
-      <c r="B76" s="87" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76" s="90">
-        <f>(C18*H18+H19*C19+C20*H20+C21*H21)</f>
-        <v>3687.3019155880088</v>
-      </c>
-      <c r="E76" s="87" t="s">
-        <v>185</v>
-      </c>
-      <c r="F76" s="90">
-        <f>(H27*C27+C28*H28+H29*C29+H30*C30)</f>
-        <v>1932.552803030303</v>
-      </c>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-    </row>
-    <row r="77" spans="2:8">
-      <c r="B77" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="C77" s="89">
-        <f>C73/1000*C74/1000*C75/1000000</f>
-        <v>1.2023808326560274E-4</v>
-      </c>
-      <c r="E77" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="F77" s="89">
-        <f>F73/1000*F74/1000*F75/1000000</f>
-        <v>1.683333165718438E-4</v>
-      </c>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
-    </row>
-    <row r="78" spans="2:8">
-      <c r="B78" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="C78" s="89">
-        <f>C77*C76</f>
-        <v>0.44335411475188752</v>
-      </c>
-      <c r="E78" s="87" t="s">
-        <v>174</v>
-      </c>
-      <c r="F78" s="89">
-        <f>F77*F76</f>
-        <v>0.32531302278430407</v>
-      </c>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
-    </row>
-    <row r="79" spans="2:8">
-      <c r="B79" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="C79" s="90">
-        <f>D18*H18+D19*H19+D20*H20</f>
-        <v>1142.1504599034699</v>
-      </c>
-      <c r="E79" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="F79" s="90">
-        <f>H27*D27+H28*D28+H29*D29</f>
-        <v>678.52884199134201</v>
-      </c>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-    </row>
-    <row r="80" spans="2:8">
-      <c r="B80" s="87" t="s">
-        <v>153</v>
-      </c>
-      <c r="C80" s="90">
-        <f>E18*H18+E19*H19+E20*H20</f>
-        <v>13.514125478652939</v>
-      </c>
-      <c r="E80" s="87" t="s">
-        <v>153</v>
-      </c>
-      <c r="F80" s="90">
-        <f>H27*E27+H28*E28+H29*E29</f>
-        <v>78.311052489177499</v>
-      </c>
-      <c r="G80" s="68"/>
-      <c r="H80" s="68"/>
-    </row>
-    <row r="81" spans="2:9">
-      <c r="B81" s="87"/>
-      <c r="C81" s="88"/>
-      <c r="E81" s="87"/>
-      <c r="F81" s="88"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-    </row>
-    <row r="82" spans="2:9">
-      <c r="B82" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="C82" s="84"/>
-      <c r="E82" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="F82" s="84"/>
-    </row>
-    <row r="83" spans="2:9">
-      <c r="B83" s="87" t="s">
-        <v>190</v>
-      </c>
-      <c r="C83" s="97">
-        <f>parameters!D13</f>
-        <v>3.54</v>
-      </c>
-      <c r="E83" s="87" t="s">
-        <v>190</v>
-      </c>
-      <c r="F83" s="97">
-        <f>parameters!K13</f>
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9">
-      <c r="B84" s="87" t="s">
-        <v>191</v>
-      </c>
-      <c r="C84" s="90">
-        <f>(C18*G18+C19*G19+C20*G20)/1000</f>
-        <v>4.0334699786758064</v>
-      </c>
-      <c r="E84" s="87" t="s">
-        <v>191</v>
-      </c>
-      <c r="F84" s="90">
-        <f>(C27*G27+C28*G28+C29*G29)/1000</f>
-        <v>2.0799099606077656</v>
-      </c>
-      <c r="G84" s="70"/>
-      <c r="H84" s="70"/>
-    </row>
-    <row r="85" spans="2:9">
-      <c r="B85" s="87" t="s">
-        <v>62</v>
-      </c>
-      <c r="C85" s="92">
-        <f>1-C83/C84</f>
-        <v>0.12234378371097065</v>
-      </c>
-      <c r="E85" s="87" t="s">
-        <v>62</v>
-      </c>
-      <c r="F85" s="92">
-        <f>1-F83/F84</f>
-        <v>0.16823322510822503</v>
-      </c>
-      <c r="G85" s="56"/>
-      <c r="H85" s="56"/>
-    </row>
-    <row r="86" spans="2:9">
-      <c r="B86" s="87"/>
-      <c r="C86" s="93"/>
-      <c r="E86" s="87"/>
-      <c r="F86" s="93"/>
-      <c r="G86" s="56"/>
-      <c r="H86" s="56"/>
-    </row>
-    <row r="87" spans="2:9">
-      <c r="B87" s="91" t="s">
-        <v>192</v>
-      </c>
-      <c r="C87" s="84"/>
-      <c r="E87" s="91" t="s">
-        <v>192</v>
-      </c>
-      <c r="F87" s="84"/>
-    </row>
-    <row r="88" spans="2:9">
-      <c r="B88" s="86" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" s="89">
-        <f>C57+C68+C77</f>
-        <v>1.3707641492278713E-4</v>
-      </c>
-      <c r="E88" s="86" t="s">
-        <v>193</v>
-      </c>
-      <c r="F88" s="89">
-        <f>F57+F68+F77</f>
-        <v>1.8517164822902819E-4</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9">
-      <c r="B89" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="C89" s="89">
-        <f>C58+C69+C78</f>
-        <v>0.48881761022628534</v>
-      </c>
-      <c r="E89" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="F89" s="89">
-        <f>F58+F69+F78</f>
-        <v>0.47685800769896347</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9">
-      <c r="B90" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="C90" s="90">
-        <f>C89/C88</f>
-        <v>3566.0227217178694</v>
-      </c>
-      <c r="E90" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="F90" s="90">
-        <f>F89/F88</f>
-        <v>2575.2214891405251</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9">
-      <c r="B91" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="C91" s="90">
-        <f>C79*(C78/$C$89)+C66*(C69/$C$89)+C55*(C58/$C$89)</f>
-        <v>1116.8385420360898</v>
-      </c>
-      <c r="E91" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="F91" s="90">
-        <f>F79*(F78/$F$89)+F66*(F69/$F$89)+F55*(F58/$F$89)</f>
-        <v>583.97448169271343</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9">
-      <c r="B92" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="C92" s="95">
-        <f>C80*(C78/$C$89)+C67*(C69/$C$89)+C56*(C58/$C$89)</f>
-        <v>30.858630944435109</v>
-      </c>
-      <c r="E92" s="94" t="s">
-        <v>197</v>
-      </c>
-      <c r="F92" s="95">
-        <f>F80*(F78/$F$89)+F67*(F69/$F$89)+F56*(F58/$F$89)</f>
-        <v>174.18749004773349</v>
-      </c>
-    </row>
-    <row r="95" spans="2:9">
-      <c r="B95" s="50" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9">
-      <c r="C96" t="s">
-        <v>199</v>
-      </c>
-      <c r="D96" t="s">
-        <v>200</v>
-      </c>
-      <c r="E96" t="s">
-        <v>201</v>
-      </c>
-      <c r="F96" t="s">
-        <v>202</v>
-      </c>
-      <c r="G96" t="s">
-        <v>42</v>
-      </c>
-      <c r="H96" t="s">
-        <v>68</v>
-      </c>
-      <c r="I96" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9">
-      <c r="C97" t="s">
-        <v>203</v>
-      </c>
-      <c r="D97" t="s">
-        <v>204</v>
-      </c>
-      <c r="E97" t="s">
-        <v>135</v>
-      </c>
-      <c r="F97" t="s">
-        <v>135</v>
-      </c>
-      <c r="G97" t="s">
-        <v>36</v>
-      </c>
-      <c r="H97" t="s">
-        <v>73</v>
-      </c>
-      <c r="I97" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9">
-      <c r="B98" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="64">
-        <f>C88</f>
-        <v>1.3707641492278713E-4</v>
-      </c>
-      <c r="D98" s="64">
-        <f>C89</f>
-        <v>0.48881761022628534</v>
-      </c>
-      <c r="E98" s="53">
-        <f>D98/SUM($D$98:$D$101)</f>
-        <v>0.46979865519035813</v>
-      </c>
-      <c r="F98" s="53">
-        <f>C98/SUM($C$98:$C$101)</f>
-        <v>0.38005202036207025</v>
-      </c>
-      <c r="G98" s="53">
-        <f>C90</f>
-        <v>3566.0227217178694</v>
-      </c>
-      <c r="H98" s="53">
-        <f>C91</f>
-        <v>1116.8385420360898</v>
-      </c>
-      <c r="I98" s="53">
-        <f>C92</f>
-        <v>30.858630944435109</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9">
-      <c r="B99" t="s">
-        <v>59</v>
-      </c>
-      <c r="C99" s="64">
-        <f>F88</f>
-        <v>1.8517164822902819E-4</v>
-      </c>
-      <c r="D99" s="64">
-        <f>F89</f>
-        <v>0.47685800769896347</v>
-      </c>
-      <c r="E99" s="53">
-        <f>D99/SUM($D$98:$D$101)</f>
-        <v>0.45830437784354566</v>
-      </c>
-      <c r="F99" s="53">
-        <f>C99/SUM($C$98:$C$101)</f>
-        <v>0.51339874232089977</v>
-      </c>
-      <c r="G99" s="53">
-        <f>F90</f>
-        <v>2575.2214891405251</v>
-      </c>
-      <c r="H99" s="53">
-        <f>F91</f>
-        <v>583.97448169271343</v>
-      </c>
-      <c r="I99" s="53">
-        <f>F92</f>
-        <v>174.18749004773349</v>
-      </c>
-    </row>
-    <row r="100" spans="2:9">
-      <c r="B100" t="s">
-        <v>97</v>
-      </c>
-      <c r="C100" s="64">
-        <f>C73/1000*C74/1000*G36/1000000</f>
-        <v>2.1041664571480475E-5</v>
-      </c>
-      <c r="D100" s="64">
-        <f>C36*C100</f>
-        <v>2.7859163892640149E-2</v>
-      </c>
-      <c r="E100" s="53">
-        <f>D100/SUM($D$98:$D$101)</f>
-        <v>2.677521729512013E-2</v>
-      </c>
-      <c r="F100" s="53">
-        <f>C100/SUM($C$98:$C$101)</f>
-        <v>5.8339190856987952E-2</v>
-      </c>
-      <c r="G100" s="53">
-        <f>C36</f>
-        <v>1324</v>
-      </c>
-      <c r="H100" s="53">
-        <f>D36</f>
-        <v>2000</v>
-      </c>
-      <c r="I100" s="53">
-        <f>E36</f>
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="101" spans="2:9">
-      <c r="B101" t="s">
-        <v>167</v>
-      </c>
-      <c r="C101" s="64">
-        <f>C45</f>
-        <v>1.7388304700256E-5</v>
-      </c>
-      <c r="D101" s="64">
-        <f>C46</f>
-        <v>4.6948422690691202E-2</v>
-      </c>
-      <c r="E101" s="53">
-        <f>D101/SUM($D$98:$D$101)</f>
-        <v>4.5121749670976118E-2</v>
-      </c>
-      <c r="F101" s="53">
-        <f>C101/SUM($C$98:$C$101)</f>
-        <v>4.8210046460042094E-2</v>
-      </c>
-      <c r="G101" s="53">
-        <f>C42</f>
-        <v>2700</v>
-      </c>
-      <c r="H101" s="53">
-        <f>C43</f>
-        <v>870</v>
-      </c>
-      <c r="I101" s="53">
-        <f>C44</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="102" spans="2:9" ht="16" thickBot="1">
-      <c r="E102" s="70"/>
-    </row>
-    <row r="103" spans="2:9">
-      <c r="B103" s="71" t="s">
-        <v>205</v>
-      </c>
-      <c r="C103" s="72">
-        <f>MAX(C62,F62)/C5</f>
-        <v>62.493806271103281</v>
-      </c>
-      <c r="D103" s="73"/>
-      <c r="E103" s="70"/>
-    </row>
-    <row r="104" spans="2:9">
-      <c r="B104" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="C104" s="75">
-        <f>C73*C74/1000/1000</f>
-        <v>0.84166658285921903</v>
-      </c>
-      <c r="D104" s="76" t="s">
-        <v>34</v>
-      </c>
-      <c r="E104" s="70"/>
-    </row>
-    <row r="105" spans="2:9">
-      <c r="B105" s="74" t="s">
-        <v>206</v>
-      </c>
-      <c r="C105" s="75">
-        <f>C64+C75+F64+F75+G36</f>
-        <v>407.85714285714289</v>
-      </c>
-      <c r="D105" s="76" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="106" spans="2:9" ht="30" customHeight="1">
-      <c r="B106" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="C106" s="69">
-        <f>C105*C103/1000</f>
-        <v>25.488545271999985</v>
-      </c>
-      <c r="D106" s="76" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="107" spans="2:9" ht="30">
-      <c r="B107" s="80" t="s">
-        <v>209</v>
-      </c>
-      <c r="C107" s="69">
-        <f>C106+2*C41</f>
-        <v>26.488545271999985</v>
-      </c>
-      <c r="D107" s="76" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="108" spans="2:9">
-      <c r="B108" s="74" t="s">
-        <v>210</v>
-      </c>
-      <c r="C108" s="69">
-        <f>E98*H98+E99*H99+E100*H100+E101*H101</f>
-        <v>885.13366342599079</v>
-      </c>
-      <c r="D108" s="76" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="109" spans="2:9">
-      <c r="B109" s="74" t="s">
-        <v>211</v>
-      </c>
-      <c r="C109" s="69">
-        <f>F98*G98+F99*G99+F100*G100+F101*G101</f>
-        <v>2884.7978279051908</v>
-      </c>
-      <c r="D109" s="76" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="110" spans="2:9" ht="30">
-      <c r="B110" s="80" t="s">
-        <v>212</v>
-      </c>
-      <c r="C110" s="69">
-        <f>E98*I98+E99*I99+E100*I100+E101*I101</f>
-        <v>103.37480593771667</v>
-      </c>
-      <c r="D110" s="76" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="111" spans="2:9" ht="16" thickBot="1">
-      <c r="B111" s="77" t="s">
-        <v>213</v>
-      </c>
-      <c r="C111" s="78">
-        <f>SUM(D98:D101)</f>
-        <v>1.0404832045085801</v>
-      </c>
-      <c r="D111" s="79" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="E48:F48"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>